<commit_message>
counting toots functionality added
</commit_message>
<xml_diff>
--- a/repository/toots_historical.xlsx
+++ b/repository/toots_historical.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E321"/>
+  <dimension ref="A1:E481"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7595,6 +7595,3638 @@
         </is>
       </c>
     </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>1.118528702093996e+17</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D322" s="2" t="n">
+        <v>45322.92769167824</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Η Adele στο Μόναχο το καλοκαίρι για τέσσερις ξεχωριστές συναυλίες &lt;a href="https://my24group.com/i-adele-sto-monacho-to-kalokairi-gia-tesseris-xechoristes-synaylies/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/i-adele-sto-mona&lt;/span&gt;&lt;span class="invisible"&gt;cho-to-kalokairi-gia-tesseris-xechoristes-synaylies/&lt;/span&gt;&lt;/a&gt; Mετά το τέλος των παρασ&amp;amp;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>1.118528701814488e+17</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>XavierMBB</t>
+        </is>
+      </c>
+      <c r="D323" s="2" t="n">
+        <v>45322.92733796296</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;𝗪𝗮𝗿𝗺𝗶𝗻𝗴 𝘂𝗽 🔥&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>1.118528701642848e+17</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>satpalram</t>
+        </is>
+      </c>
+      <c r="D324" s="2" t="n">
+        <v>45322.92767361111</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;All our Tierneys come at once. &lt;a href="https://mastodonapp.uk/tags/LFC" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;LFC&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>1.118528701604128e+17</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>MLS</t>
+        </is>
+      </c>
+      <c r="D325" s="2" t="n">
+        <v>45322.92631944444</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Fresh off a record-breaking expansion season, &lt;span class="h-card"&gt;&lt;a href="https://twitter.com/stlCITYsc" class="u-url mention" rel="nofollow noopener noreferrer" target="_blank"&gt;@&lt;span&gt;stlCITYsc@sportsbots.xyz&lt;/span&gt;&lt;/a&gt;&lt;/span&gt; have signed head coach Bradley Carnell to a contract extension. ✍️&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>1.118528701439985e+17</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>hkrn</t>
+        </is>
+      </c>
+      <c r="D326" s="2" t="n">
+        <v>45322.92765046296</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Executing Cron Scripts Reliably at Scale&lt;br&gt;L: &lt;a href="https://slack.engineering/executing-cron-scripts-reliably-at-scale/" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;slack.engineering/executing-cr&lt;/span&gt;&lt;span class="invisible"&gt;on-scripts-reliably-at-scale/&lt;/span&gt;&lt;/a&gt;&lt;br&gt;C: &lt;a href="https://news.ycombinator.com/item?id=39173665" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;news.ycombinator.com/item?id=3&lt;/span&gt;&lt;span class="invisible"&gt;9173665&lt;/span&gt;&lt;/a&gt;&lt;br&gt;posted on 2024.01.29 at 02:21:58 (c=0, p=3)&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>1.118528701430961e+17</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>l_l_bryant</t>
+        </is>
+      </c>
+      <c r="D327" s="2" t="n">
+        <v>45322.92767361111</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;- ZZZ looks like it could be fun, but I need to see more.&lt;br&gt;- Foamstars not my cup of tea.&lt;br&gt;- Dave the Diver - good catch for Sony.&lt;/p&gt;&lt;p&gt;&lt;a href="https://mstdn.games/tags/stateofplay" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;stateofplay&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>1.118528701337861e+17</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>memeorandum</t>
+        </is>
+      </c>
+      <c r="D328" s="2" t="n">
+        <v>45322.92765046296</v>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Pro-Palestinian Activists Were Denied Entry to a Kamala Harris Event, Accused the Organizers of Racism (John Sexton/HotAir)&lt;/p&gt;&lt;p&gt;&lt;a href="https://hotair.com/john-s-2/2024/01/31/pro-palestinian-activists-were-denied-entry-to-a-kamala-harris-event-accused-the-organizers-of-racism-n608687" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;hotair.com/john-s-2/2024/01/31&lt;/span&gt;&lt;span class="invisible"&gt;/pro-palestinian-activists-were-denied-entry-to-a-kamala-harris-event-accused-the-organizers-of-racism-n608687&lt;/span&gt;&lt;/a&gt;&lt;br&gt;&lt;a href="http://www.memeorandum.com/240131/p86#a240131p86" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;http://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;memeorandum.com/240131/p86#a24&lt;/span&gt;&lt;span class="invisible"&gt;0131p86&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>1.118528701253102e+17</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>BethanyBlack</t>
+        </is>
+      </c>
+      <c r="D329" s="2" t="n">
+        <v>45322.92767680556</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;I’ve done my bit to bring down inflation and *checks notes* paying out on bonds generated to create treasury money for public services in the 1960s&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>1.118528700853671e+17</v>
+      </c>
+      <c r="B330" t="inlineStr"/>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>haohailong</t>
+        </is>
+      </c>
+      <c r="D330" s="2" t="n">
+        <v>45322.92763186343</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;在听 &lt;a href="https://neodb.social/~neodb~/album/0c7cEfTTvTgCskHZYoKJXi" rel="nofollow noopener noreferrer" target="_blank"&gt;Please Please Me&lt;/a&gt; &lt;/p&gt;&lt;p&gt;&lt;a href="https://neodb.social/tags/我的書影音/" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#我的書影音&lt;/a&gt; &lt;a href="https://neodb.social/tags/我的书影音/" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#我的书影音&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>1.118528700809417e+17</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>jepyang</t>
+        </is>
+      </c>
+      <c r="D331" s="2" t="n">
+        <v>45322.92760416667</v>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Real life should be more like Monopoly&lt;/p&gt;&lt;p&gt;(I should receive $200 every ten minutes simply for continuing to exist)&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>1.118528700639924e+17</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>McRaeWrites</t>
+        </is>
+      </c>
+      <c r="D332" s="2" t="n">
+        <v>45322.92766600694</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Broken Savant Syndrome.&lt;/p&gt;&lt;p&gt;&lt;a href="https://mcraewrites.com/broken-savant-syndrome/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;mcraewrites.com/broken-savant-&lt;/span&gt;&lt;span class="invisible"&gt;syndrome/&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>1.118528700354458e+17</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>futpicante</t>
+        </is>
+      </c>
+      <c r="D333" s="2" t="n">
+        <v>45322.92649305556</v>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;¡SUBASTARÁN la servilleta que cambió la vida de MESSI! &lt;/p&gt;&lt;p&gt;💥 👀 👇&lt;/p&gt;&lt;p&gt;&lt;a href="https://www.espn.com.mx/futbol/espana/nota/_/id/13169846/saldra-a-subasta-la-servilleta-que-cambio-la-vida-de-messi" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;espn.com.mx/futbol/espana/…&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>1.118528700328545e+17</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>verdantsquare</t>
+        </is>
+      </c>
+      <c r="D334" s="2" t="n">
+        <v>45322.9275</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Bird flu viruses may pack tools that help them infect human cells - Science News Magazine &lt;a href="https://news.google.com/rss/articles/CBMiS2h0dHBzOi8vd3d3LnNjaWVuY2VuZXdzLm9yZy9hcnRpY2xlL2hvdy1iaXJkLWZsdS12aXJ1c2VzLWluZmVjdC1odW1hbi1jZWxsc9IBAA?oc=5&amp;amp;utm_source=dlvr.it&amp;amp;utm_medium=mastodon" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;news.google.com/rss/articles/C&lt;/span&gt;&lt;span class="invisible"&gt;BMiS2h0dHBzOi8vd3d3LnNjaWVuY2VuZXdzLm9yZy9hcnRpY2xlL2hvdy1iaXJkLWZsdS12aXJ1c2VzLWluZmVjdC1odW1hbi1jZWxsc9IBAA?oc=5&amp;amp;utm_source=dlvr.it&amp;amp;utm_medium=mastodon&lt;/span&gt;&lt;/a&gt; &lt;a href="https://gratefuldread.masto.host/tags/science" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;science&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>1.11852870026615e+17</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>ru</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>meduza_unshackled</t>
+        </is>
+      </c>
+      <c r="D335" s="2" t="n">
+        <v>45322.92765046296</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;✹ Все музыканты «Би-2», задержанные 24 января на Пхукете, вылетели из Таиланда в Израиль.&lt;/p&gt;&lt;p&gt;✹ Госдума приняла закон о&amp;nbsp;конфискации имущества за&amp;nbsp;«фейки» об&amp;nbsp;армии.&lt;/p&gt;&lt;p&gt;✹ Борис Надеждин сдал в&amp;nbsp;ЦИК подписи для выдвижения в&amp;nbsp;президенты.&lt;/p&gt;&lt;p&gt;✹ Россия и Украина провели первый обмен пленными после катастрофы Ил-76. В Россию вернулись 195 военнослужащих, в Украину — 207 военных и гражданских.&lt;/p&gt;&lt;p&gt;✹ В Лондоне задержали бывшего губернатора аннексированного Севастополя Дмитрия Овсянникова по&amp;nbsp;делу о&amp;nbsp;нарушении санкций. В&amp;nbsp;2022 году он&amp;nbsp;добился снятия санкций ЕС.&lt;/p&gt;&lt;p&gt;———&lt;/p&gt;&lt;p&gt;Текст дня: «Крутые все». «Медуза» рассказывает, что известно о каждом участнике группы «Би-2» (спойлер: среди них основатель Planeta.ru, самый известный прог-музыкант страны и&amp;nbsp;флейтист «Сплина»). Российские власти требовали от Таиланда их депортации, но в итоге музыкантам удалось избежать этого и улететь в Израиль.&lt;/p&gt;&lt;p&gt;🔗 &lt;a href="https://t.me/meduzalive/99308" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;t.me/meduzalive/99308&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>1.118528700239862e+17</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>roboaqraf</t>
+        </is>
+      </c>
+      <c r="D336" s="2" t="n">
+        <v>45322.92763888889</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;車借りたらシュッと移動しないと満足に動かない &lt;a href="https://m.aqr.af/tags/bot" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;bot&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>1.118528700173661e+17</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D337" s="2" t="n">
+        <v>45322.92765896991</v>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;ΗΠΑ: Η Fed διατηρεί τα επιτόκιά της, δεν προβλέπει ακόμη τη μείωσή τους &lt;a href="https://my24group.com/ipa-i-fed-diatirei-ta-epitokia-tis-den-provlepei-akomi-ti-meiosi-toys/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/ipa-i-fed-diatir&lt;/span&gt;&lt;span class="invisible"&gt;ei-ta-epitokia-tis-den-provlepei-akomi-ti-meiosi-toys/&lt;/span&gt;&lt;/a&gt; Η αμερικανική κεντρικ&amp;amp;#94…&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>1.118528699924919e+17</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>kakopon</t>
+        </is>
+      </c>
+      <c r="D338" s="2" t="n">
+        <v>45322.92765342593</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://mastodon.social/tags/%E7%A6%8F%E5%B1%B1%E5%92%8C%E4%BA%BA%E3%81%95%E3%82%93%E3%82%92%E4%BA%AC%E9%83%BD%E5%B8%82%E9%95%B7%E3%81%AB" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;福山和人さんを京都市長に&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>1.118528699883482e+17</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>claralistensprechen3rd</t>
+        </is>
+      </c>
+      <c r="D339" s="2" t="n">
+        <v>45322.92741898148</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://friendica.myportal.social/search?tag=WingedWednesday" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;WingedWednesday&lt;/span&gt;&lt;/a&gt; &lt;a href="https://friendica.myportal.social/search?tag=MyPhoto" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;MyPhoto&lt;/span&gt;&lt;/a&gt; &lt;a href="https://friendica.myportal.social/search?tag=MyWork" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;MyWork&lt;/span&gt;&lt;/a&gt; &lt;a href="https://friendica.myportal.social/search?tag=nature" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;nature&lt;/span&gt;&lt;/a&gt; &lt;a href="https://friendica.myportal.social/search?tag=butterflies" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;butterflies&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Red Admiral peers down from a blooming apricot twig.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>1.118528699579798e+17</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>mikemathia</t>
+        </is>
+      </c>
+      <c r="D340" s="2" t="n">
+        <v>45322.92759259259</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;It's a photo of meeeee&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>1.118528699509213e+17</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>wlaatje</t>
+        </is>
+      </c>
+      <c r="D341" s="2" t="n">
+        <v>45322.92759259259</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;[🚨series spoiler alert🚨]&lt;/p&gt;&lt;p&gt;Winnner of the Best Supporting Actress for the: &lt;br&gt;🏆 Golden Globes 2024&lt;br&gt;🏆 Emmy Award 2024&lt;br&gt;🏆 Oscar 2024&lt;/p&gt;&lt;p&gt;👉 Jennifer Jason Leigh&lt;/p&gt;&lt;p&gt;&lt;a href="https://social.edu.nl/tags/LorraineLyon" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;LorraineLyon&lt;/span&gt;&lt;/a&gt; &lt;a href="https://social.edu.nl/tags/Fargo" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Fargo&lt;/span&gt;&lt;/a&gt; &lt;a href="https://social.edu.nl/tags/S05" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;S05&lt;/span&gt;&lt;/a&gt; &lt;a href="https://social.edu.nl/tags/recommendation" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;recommendation&lt;/span&gt;&lt;/a&gt; &lt;a href="https://social.edu.nl/tags/donedeal" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;donedeal&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>1.118528699168537e+17</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D342" s="2" t="n">
+        <v>45322.92764002315</v>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Υποκλίθηκε στην Τενερίφη το Περιστέρι &lt;a href="https://my24group.com/ypoklithike-stin-tenerifi-to-peristeri/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/ypoklithike-stin&lt;/span&gt;&lt;span class="invisible"&gt;-tenerifi-to-peristeri/&lt;/span&gt;&lt;/a&gt;   Οι “πρίγκιπες της δυ&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>1.118528698954724e+17</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>tako800</t>
+        </is>
+      </c>
+      <c r="D343" s="2" t="n">
+        <v>45322.92760416667</v>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;リマスタードット、セシルはリマスター感あるけど、バッツとティナはオリジナルのが良いような気がしてしまうな🐴&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>1.118528698879492e+17</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>haohailong</t>
+        </is>
+      </c>
+      <c r="D344" s="2" t="n">
+        <v>45322.92763503472</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;在听《Please Please Me》&lt;br /&gt;&lt;a href="https://neodb.social/album/0c7cEfTTvTgCskHZYoKJXi" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;neodb.social/album/0c7cEfTTvTg&lt;/span&gt;&lt;span class="invisible"&gt;CskHZYoKJXi&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://mastodon.social/tags/%E6%88%91%E7%9A%84%E6%9B%B8%E5%BD%B1%E9%9F%B3" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;我的書影音&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/%E6%88%91%E7%9A%84%E4%B9%A6%E5%BD%B1%E9%9F%B3" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;我的书影音&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>1.118528698743541e+17</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>YvanDutil</t>
+        </is>
+      </c>
+      <c r="D345" s="2" t="n">
+        <v>45322.92756944444</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Projet de recherche ciel étoilé à St-Camille &lt;a href="https://ici.radio-canada.ca/ohdio/premiere/emissions/Par-ici-l-info/segments/rattrapage/473709/projet-de-recherche-ciel-etoile-a-st-camille" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;ici.radio-canada.ca/ohdio/prem&lt;/span&gt;&lt;span class="invisible"&gt;iere/emissions/Par-ici-l-info/segments/rattrapage/473709/projet-de-recherche-ciel-etoile-a-st-camille&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>1.118528698729618e+17</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Bahdlex</t>
+        </is>
+      </c>
+      <c r="D346" s="2" t="n">
+        <v>45322.92763229166</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Actress, Omoni Oboli&amp;#39;s son, Tobe is engaged. 🥰&lt;br /&gt;.&lt;br /&gt;&lt;a href="https://mastodon.social/tags/bahdlex" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;bahdlex&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/OmoniOboli" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;OmoniOboli&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>1.118528698622338e+17</v>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>BrianMFloyd</t>
+        </is>
+      </c>
+      <c r="D347" s="2" t="n">
+        <v>45322.92724537037</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;its easy to see why they like the big gun that goes brrrrrrrrrt and also why its never a good sign when they have to use it&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>1.118528698613124e+17</v>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>ciredutempsEsme</t>
+        </is>
+      </c>
+      <c r="D348" s="2" t="n">
+        <v>45322.92760416667</v>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://mamot.fr/tags/passionZeugme" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;passionZeugme&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>1.118528698386968e+17</v>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>uk</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>MAKS23</t>
+        </is>
+      </c>
+      <c r="D349" s="2" t="n">
+        <v>45322.9276262037</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;❗️ UNCONFIRMED information from Russian telegram channel. &lt;/p&gt;&lt;p&gt;🇺🇦 AFU expanded the bridgehead in Krynki&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>1.118528698332399e+17</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D350" s="2" t="n">
+        <v>45322.92762525463</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Angi: Making Progress Reducing Losses &lt;a href="https://my24group.com/angi-making-progress-reducing-losses/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/angi-making-prog&lt;/span&gt;&lt;span class="invisible"&gt;ress-reducing-losses/&lt;/span&gt;&lt;/a&gt;   Read More &lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>1.118528698172196e+17</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>theblindarcher</t>
+        </is>
+      </c>
+      <c r="D351" s="2" t="n">
+        <v>45322.92761574074</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;One of my current comms is a Fortnite portrait set...&lt;/p&gt;&lt;p&gt;I knew what I was getting myself into, and I still get surprised somehow 💀&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>1.118528698104589e+17</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>TheEuropeanLad</t>
+        </is>
+      </c>
+      <c r="D352" s="2" t="n">
+        <v>45322.9258912037</v>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;FT: Liverpool 4-1 Chelsea.&lt;/p&gt;&lt;p&gt;Liverpool remain 1st! Chelsea go back in 10th!&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>1.11852869807782e+17</v>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D353" s="2" t="n">
+        <v>45322.92762076389</v>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;US-Zinsentscheid: Fed fordert Geduld von Investoren – Börsen reagieren deutlich &lt;a href="https://my24group.com/us-zinsentscheid-fed-fordert-geduld-von-investoren-borsen-reagieren-deutlich/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/us-zinsentscheid&lt;/span&gt;&lt;span class="invisible"&gt;-fed-fordert-geduld-von-investoren-borsen-reagieren-deutlich/&lt;/span&gt;&lt;/a&gt; Die US-Notenbank hält die Zinsen auf höchstem Stand seit 23 Jahren und stellt Senkungen „irgendwann in die…&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>1.118528697908706e+17</v>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D354" s="2" t="n">
+        <v>45322.9276177662</v>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Florida judge dismisses Disney’s free-speech case against Ron DeSantis &lt;a href="https://my24group.com/florida-judge-dismisses-disneys-free-speech-case-against-ron-desantis/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/florida-judge-di&lt;/span&gt;&lt;span class="invisible"&gt;smisses-disneys-free-speech-case-against-ron-desantis/&lt;/span&gt;&lt;/a&gt; Company vows ‘case will not end here’ in feud that started when it opposed Republican governor’s ‘&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>1.118528697675983e+17</v>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>factline</t>
+        </is>
+      </c>
+      <c r="D355" s="2" t="n">
+        <v>45322.92759259259</v>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Bosses from five of the largest social media firms were grilled about how they are protecting children. Read More BBC News – World … &lt;br&gt;&lt;a href="https://factline.org/meta-boss-mark-zuckerberg-apologises-to-families-in-fiery-us-senate-hearing/" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;factline.org/meta-boss-mark-zu&lt;/span&gt;&lt;span class="invisible"&gt;ckerberg-apologises-to-families-in-fiery-us-senate-hearing/&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>1.118528697608699e+17</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D356" s="2" t="n">
+        <v>45322.92761248843</v>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Streik: Warnstreik an Airports gestartet – hunderte Flugausfälle &lt;a href="https://my24group.com/streik-warnstreik-an-airports-gestartet-hunderte-flugausfalle/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/streik-warnstrei&lt;/span&gt;&lt;span class="invisible"&gt;k-an-airports-gestartet-hunderte-flugausfalle/&lt;/span&gt;&lt;/a&gt; Durch einen Warnstreik an großen deutschen Airports kommt es zu hunderten Flugausfällen. Am Flughafen Köln…&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>1.118528696923719e+17</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>jamiecrook</t>
+        </is>
+      </c>
+      <c r="D357" s="2" t="n">
+        <v>45322.92759259259</v>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;I don’t think any of us expected it, but Conor Bradley has cemented his place in the team for now. Phenomenal performance at both ends of the pitch. &lt;a href="https://mastodonapp.uk/tags/LFC" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;LFC&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>1.118528696858107e+17</v>
+      </c>
+      <c r="B358" t="inlineStr"/>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>jemibiozoms</t>
+        </is>
+      </c>
+      <c r="D358" s="2" t="n">
+        <v>45322.92758355324</v>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;span&gt;キャラデザ苦手丸なので先に性格がガチガチに固まってしまうけどそうなると余計にビジュアルがその性格らしくならないと無理になるので難易度が上がってしまう現象&lt;/span&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>1.118528696691957e+17</v>
+      </c>
+      <c r="B359" t="inlineStr"/>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>eythian</t>
+        </is>
+      </c>
+      <c r="D359" s="2" t="n">
+        <v>45322.92752600695</v>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>Robin started reading &lt;a href="https://bookwyrm.social/book/1207650" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;i&gt;The Count of Monte Christo&lt;/i&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>1.118528696210594e+17</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>SJohnsonSport</t>
+        </is>
+      </c>
+      <c r="D360" s="2" t="n">
+        <v>45322.92585648148</v>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;That’s it. &lt;a href="https://twitter.com/hashtag/CFC" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;CFC&lt;/span&gt;&lt;/a&gt; lose 4-1. Another terrible display away from home. &lt;a href="https://twitter.com/hashtag/LIVCHE" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;LIVCHE&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>1.118528696031492e+17</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>theusasingers</t>
+        </is>
+      </c>
+      <c r="D361" s="2" t="n">
+        <v>45322.92758467593</v>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;It’s not enough to just beat Trump in November, we must summon an epic Blue Wave &amp;amp; humiliate him.&lt;/p&gt;&lt;p&gt;We need so show the MAGA cult that we are indeed the majority.&lt;/p&gt;&lt;p&gt;We have to crush him in a historic landslide which will put to rest his reign of terror once &amp;amp; for all.&lt;/p&gt;&lt;p&gt;Vote Blue.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>1.118528716989748e+17</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>jbzfn</t>
+        </is>
+      </c>
+      <c r="D362" s="2" t="n">
+        <v>45322.92795476852</v>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Permission to rename this curse to &amp;quot;MLLM&amp;quot;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>1.11852871691999e+17</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>zh-CN</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>cosmicraven</t>
+        </is>
+      </c>
+      <c r="D363" s="2" t="n">
+        <v>45322.92792824074</v>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;做实验是一种禅修，真的。&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>1.118528716761277e+17</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>MrKrisKrisu</t>
+        </is>
+      </c>
+      <c r="D364" s="2" t="n">
+        <v>45322.92792824074</v>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Ich muss mal wieder mehr privat auf Reisen gehen. :breadpeek:&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>1.118528716639435e+17</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>smithmeyerjen</t>
+        </is>
+      </c>
+      <c r="D365" s="2" t="n">
+        <v>45322.9278125</v>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Wordle 957 4/6&lt;/p&gt;&lt;p&gt;⬜⬜⬜⬜🟩&lt;br&gt;⬜⬜🟨⬜🟩&lt;br&gt;⬜🟩🟨⬜🟩&lt;br&gt;🟩🟩🟩🟩🟩&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>1.118528716623411e+17</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>bencgtravels</t>
+        </is>
+      </c>
+      <c r="D366" s="2" t="n">
+        <v>45322.92794833333</v>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Blimey, it&amp;#39;s a &amp;#39;Shadow the Hedgehog&amp;#39; (2005) remake supposedly without the guns, (thank god) packed in with a spruced up Sonic Generations? That&amp;#39;s an unexpected project to get greenlighted. Definitely seems like part of &amp;#39;Project clean up the lore.&amp;#39;&lt;br /&gt;&lt;a href="https://youtu.be/CDmVayEU76w?si=KbUyVuOfXTO5gtfK" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;youtu.be/CDmVayEU76w?si=KbUyVu&lt;/span&gt;&lt;span class="invisible"&gt;OfXTO5gtfK&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>1.118528716376124e+17</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>pubx</t>
+        </is>
+      </c>
+      <c r="D367" s="2" t="n">
+        <v>45322.92788194444</v>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://www.pub-x.com/318511/" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class=""&gt;pub-x.com/318511/&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt; 240131 WE_NMIXX キュジンのTwitter更新 &lt;a href="https://jforo.com/tags/NMIXX" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NMIXX&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>1.118528716071885e+17</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D368" s="2" t="n">
+        <v>45322.92765046296</v>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;You know you're onto a good then when you walk into the cafe and the barista immediately calls you over to show you a picture of a t-shirt covered in chihuahuas, and you then text them a photo of your dog because they've been telling their friends about her.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>1.118528715251083e+17</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>death.au</t>
+        </is>
+      </c>
+      <c r="D369" s="2" t="n">
+        <v>45322.92791666667</v>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>I kinda want to write blog posts, but I don't really know what I want to write about ¯_(ツ)_/¯</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="n">
+        <v>1.118528715021229e+17</v>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>europesays</t>
+        </is>
+      </c>
+      <c r="D370" s="2" t="n">
+        <v>45322.9278587963</v>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://www.europesays.com/1031608/" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class=""&gt;europesays.com/1031608/&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt; Quand Amélie Oudéa-Castéra s’activait au service d’une école privée hors contrat &lt;a href="https://pubeurope.com/tags/france" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;france&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="n">
+        <v>1.118528714948888e+17</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>geist</t>
+        </is>
+      </c>
+      <c r="D371" s="2" t="n">
+        <v>45322.92790509259</v>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Snaaaake Pliskon bleibt der schärfste.&lt;br&gt;Wenn du mit soner Peter Maffay Matte Karriere schaffst, gehörst du eif. zu den Besten!&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="n">
+        <v>1.118528714599901e+17</v>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>civfanatics</t>
+        </is>
+      </c>
+      <c r="D372" s="2" t="n">
+        <v>45322.92789351852</v>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://www.youtube.com/watch?v=bo31IW0CWPI" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;youtube.com/watch?v=bo31IW0CWP&lt;/span&gt;&lt;span class="invisible"&gt;I&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;And we are now at the 16th dev diary for &lt;a href="https://mstdn.games/tags/Ara" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Ara&lt;/span&gt;&lt;/a&gt;: History Untold.&lt;br&gt;This time the devs talk about gaming the art in the game. They talk about how to choose the style for a game, how to properly represent cultures and how they try to give a customized style for each new play of the game.&lt;/p&gt;&lt;p&gt;The game:&lt;br&gt;- &lt;a href="https://www.arahistoryuntold.com/" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class=""&gt;arahistoryuntold.com/&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Our thread:&lt;br&gt;- &lt;a href="https://forums.civfanatics.com/threads/ara-history-untold.677325/page-13#post-16561596" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;forums.civfanatics.com/threads&lt;/span&gt;&lt;span class="invisible"&gt;/ara-history-untold.677325/page-13#post-16561596&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="n">
+        <v>1.118528714268906e+17</v>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>mmorpg</t>
+        </is>
+      </c>
+      <c r="D373" s="2" t="n">
+        <v>45322.92787037037</v>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Today @NewsBlackDesert opens the new Yzrahid Highlands monster zone, adds the War of the Roses main questline, new Academia costume, and continues streamlining features to improve the player experience.&amp;nbsp; &lt;br&gt;&lt;a href="https://www.mmorpg.com/news/black-desert-online-adds-new-high-level-monster-zone-war-of-the-roses-questline-and-300-person-pvp-mode-2000130311" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;mmorpg.com/news/black-desert-o&lt;/span&gt;&lt;span class="invisible"&gt;nline-adds-new-high-level-monster-zone-war-of-the-roses-questline-and-300-person-pvp-mode-2000130311&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Original tweet : &lt;a href="https://twitter.com/MMORPGcom/status/1752735266790408297" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;twitter.com/MMORPGcom/status/1&lt;/span&gt;&lt;span class="invisible"&gt;752735266790408297&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="n">
+        <v>1.118528714009853e+17</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>nl</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>StellaQuasten</t>
+        </is>
+      </c>
+      <c r="D374" s="2" t="n">
+        <v>45322.92788194444</v>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Mooi zo, want moet zeker twee wassen draaien 😅&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="n">
+        <v>1.118528713937895e+17</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>PetaPixel</t>
+        </is>
+      </c>
+      <c r="D375" s="2" t="n">
+        <v>45322.92711805556</v>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Viltrox’s AF 20mm f/2.8 is Now Available for Nikon Z-Mount &lt;a href="https://petapixel.com/2024/01/31/viltroxs-af-20mm-f-2-8-is-now-available-for-nikon-z-mount/" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;petapixel.com/2024/01/31/viltr&lt;/span&gt;&lt;span class="invisible"&gt;oxs-af-20mm-f-2-8-is-now-available-for-nikon-z-mount/&lt;/span&gt;&lt;/a&gt; &lt;a href="https://toot.earth/tags/viltroxaf20mmf28" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;viltroxaf20mmf28&lt;/span&gt;&lt;/a&gt; &lt;a href="https://toot.earth/tags/nikonzmount" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;nikonzmount&lt;/span&gt;&lt;/a&gt; &lt;a href="https://toot.earth/tags/emountlens" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;emountlens&lt;/span&gt;&lt;/a&gt; &lt;a href="https://toot.earth/tags/Equipment" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Equipment&lt;/span&gt;&lt;/a&gt; &lt;a href="https://toot.earth/tags/20mmf28" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;20mmf28&lt;/span&gt;&lt;/a&gt; &lt;a href="https://toot.earth/tags/viltrox" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;viltrox&lt;/span&gt;&lt;/a&gt; &lt;a href="https://toot.earth/tags/News" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;News&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="n">
+        <v>1.118528713784743e+17</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>lcrmx</t>
+        </is>
+      </c>
+      <c r="D376" s="2" t="n">
+        <v>45322.9278587963</v>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>Alertan llegada "con fuerza" de subvariante Pirola de Covid-19 a México &lt;a href="https://sipse.com/mexico/alertan-llegada-fuerza-subvariante-pirola-covid-19-mexico-462854.html" rel="nofollow noopener noreferrer" target="_blank"&gt;sipse.com/mexico/alertan-llega…&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="n">
+        <v>1.11852871307003e+17</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>rawchili</t>
+        </is>
+      </c>
+      <c r="D377" s="2" t="n">
+        <v>45322.9278587963</v>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;How I slept last night knowing some lakers fans spent almost a grand to buy my seats just for the privilege to watch them get blown out by the hox &lt;a href="https://www.rawchili.com/3282990/" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class=""&gt;rawchili.com/3282990/&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://channels.im/tags/Atlanta" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Atlanta&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/AtlantaHawks" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;AtlantaHawks&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/basketball" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;basketball&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/Georgia" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Georgia&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/Hawks" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Hawks&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/NationalBasketballAssociation" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NationalBasketballAssociation&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/NBA" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NBA&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/NBAEasternConference" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NBAEasternConference&lt;/span&gt;&lt;/a&gt; &lt;a href="https://channels.im/tags/NBAEasternConferenceSoutheastDivision" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NBAEasternConferenceSoutheastDivision&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="n">
+        <v>1.118528712651263e+17</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>iembot_oun</t>
+        </is>
+      </c>
+      <c r="D378" s="2" t="n">
+        <v>45322.92787037037</v>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://bots.krohsnest.com/tags/OKweather" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;OKweather&lt;/span&gt;&lt;/a&gt; &lt;a href="https://bots.krohsnest.com/tags/OKwx" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;OKwx&lt;/span&gt;&lt;/a&gt;&lt;br&gt;345 &lt;br&gt;CDUS44 KOUN 312213&lt;br&gt;CLISPS&lt;/p&gt;&lt;p&gt;CLIMATE REPORT &lt;br&gt;NATIONAL WEATHER SERVICE NORMAN OK&lt;br&gt;413 PM CST WED JAN 31 2024&lt;/p&gt;&lt;p&gt;...................................&lt;/p&gt;&lt;p&gt;...THE WICHITA FALLS CLIMATE SUMMARY FOR JANUARY 31 2024...&lt;br&gt;VALID AS OF 0400 PM LOCAL TIME.&lt;/p&gt;&lt;p&gt;CLIMATE NORMAL PERIOD 1991 TO 2020&lt;br&gt;CLIMATE RECORD PERIOD 1897 TO 2024&lt;/p&gt;&lt;p&gt;WEATHER ITEM   OBSERVED RECORD YEAR NORMAL DEPARTURE                  &lt;br&gt;                 &lt;a href="https://mesonet.agron.iastate.edu/p.php?pid=202401312213-KOUN-CDUS44-CLISPS" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;mesonet.agron.iastate.edu/p.ph&lt;/span&gt;&lt;span class="invisible"&gt;p?pid=202401312213-KOUN-CDUS44-CLISPS&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>1.118528712577578e+17</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>ko</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>news_society</t>
+        </is>
+      </c>
+      <c r="D379" s="2" t="n">
+        <v>45322.92782407408</v>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;"대규모 전세 사기 서울 화곡동 근황…충격의 경매 지도"&lt;br&gt;대규모 전세 사기가 발생한 곳이죠. 서울 강서구 화곡동의 경매 현황이 담긴 지도가 누리꾼들에게 충격을 주고 있습니다. 최근 온라인 커뮤니티에는 '화곡동 근황'이라며 경매 지도가 올라왔습니다.&lt;br&gt;&lt;a href="https://news.sbs.co.kr/news/endPage.do?news_id=N1007520799" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;news.sbs.co.kr/news/endPage.do&lt;/span&gt;&lt;span class="invisible"&gt;?news_id=N1007520799&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://802.3ether.net/tags/news" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;news&lt;/span&gt;&lt;/a&gt; &lt;a href="https://802.3ether.net/tags/%EB%89%B4%EC%8A%A4" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;뉴스&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>1.118528712332077e+17</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>ohtorifightclub</t>
+        </is>
+      </c>
+      <c r="D380" s="2" t="n">
+        <v>45322.9278587963</v>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;ayyyyy V rising&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>1.118528712298835e+17</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>austin_traffic_bot</t>
+        </is>
+      </c>
+      <c r="D381" s="2" t="n">
+        <v>45322.9278719213</v>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;COLLISION at 1915 W WELLS BRANCH PKWY --- &lt;a href="https://www.google.com/maps/search/?api=1&amp;amp;query=30.433768%2C-97.680681" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;google.com/maps/search/?api=1&amp;amp;&lt;/span&gt;&lt;span class="invisible"&gt;query=30.433768%2C-97.680681&lt;/span&gt;&lt;/a&gt; --- &lt;a href="https://mastodon.social/tags/austin" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;austin&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/austintx" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;austintx&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/traffic" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;traffic&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="n">
+        <v>1.118528712294e+17</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>Newmy</t>
+        </is>
+      </c>
+      <c r="D382" s="2" t="n">
+        <v>45322.9278587963</v>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Maybe it's just my algorithm or whatever but there is like this really pronounced strain of savvy Apple fanaticism that is weirdly like going back to late aughts Twitter all over again&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>1.118528711893103e+17</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>ranzware</t>
+        </is>
+      </c>
+      <c r="D383" s="2" t="n">
+        <v>45322.9278587963</v>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;February&amp;amp;apos;s PlayStation Plus games include Foamstars, Rollerdrome and Steelrising &lt;a href="https://ranzware.com/februarys-playstation-plus-games-include-foamstars-rollerdrome-and-steelrising" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;ranzware.com/februarys-playsta&lt;/span&gt;&lt;span class="invisible"&gt;tion-plus-games-include-foamstars-rollerdrome-and-steelrising&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>1.118528711820924e+17</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>emarktaylor</t>
+        </is>
+      </c>
+      <c r="D384" s="2" t="n">
+        <v>45322.92778935185</v>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://thecanadian.social/tags/GiantMilitaryCats" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;GiantMilitaryCats&lt;/span&gt;&lt;/a&gt; &lt;/p&gt;&lt;p&gt;Via Soft Side @SoftSide1 &lt;br&gt;·&lt;br&gt;2h&lt;br&gt;Replying to @giantcat9&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>1.118528711611773e+17</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>hypomodern</t>
+        </is>
+      </c>
+      <c r="D385" s="2" t="n">
+        <v>45322.9278125</v>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;From The Bird Place...&lt;/p&gt;&lt;p&gt;Star Trek calling shots :D&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>1.118528711461846e+17</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>pennadsb</t>
+        </is>
+      </c>
+      <c r="D386" s="2" t="n">
+        <v>45322.92778935185</v>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://airwaves.social/tags/PlaneAlert" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;PlaneAlert&lt;/span&gt;&lt;/a&gt; ICAO: &lt;a href="https://airwaves.social/tags/AE03E0" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;AE03E0&lt;/span&gt;&lt;/a&gt; Tail: #164993 Flt: &lt;a href="https://airwaves.social/tags/CNV3836" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;CNV3836&lt;/span&gt;&lt;/a&gt; &lt;br&gt;Owner: &lt;a href="https://airwaves.social/tags/USAF" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;USAF&lt;/span&gt;&lt;/a&gt;&lt;br&gt;Aircraft: &lt;a href="https://airwaves.social/tags/C" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;C&lt;/span&gt;&lt;/a&gt;-130T Hercules&lt;br&gt;2024/01/31 17:14:15&lt;br&gt;&lt;a href="https://airwaves.social/tags/C130" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;C130&lt;/span&gt;&lt;/a&gt; &lt;a href="https://airwaves.social/tags/Cargo" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Cargo&lt;/span&gt;&lt;/a&gt; &lt;a href="https://airwaves.social/tags/AbsoluteUnit" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;AbsoluteUnit&lt;/span&gt;&lt;/a&gt; &lt;a href="https://airwaves.social/tags/TacticalAirlift" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;TacticalAirlift&lt;/span&gt;&lt;/a&gt; &lt;a href="https://www.airforce.com" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class=""&gt;airforce.com&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt; &lt;br&gt;&lt;a href="https://globe.adsbexchange.com/?icao=AE03E0&amp;amp;showTrace=2024-01-31&amp;amp;zoom=7&amp;amp;lat=40.338724&amp;amp;lon=-79.388455&amp;amp;timestamp=1706739255" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;globe.adsbexchange.com/?icao=A&lt;/span&gt;&lt;span class="invisible"&gt;E03E0&amp;amp;showTrace=2024-01-31&amp;amp;zoom=7&amp;amp;lat=40.338724&amp;amp;lon=-79.388455&amp;amp;timestamp=1706739255&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>1.118528711384626e+17</v>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>infodocket</t>
+        </is>
+      </c>
+      <c r="D387" s="2" t="n">
+        <v>45322.92782407408</v>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Research Tools: UNC Collaboration to Create Public &lt;a href="https://newsie.social/tags/Depository" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Depository&lt;/span&gt;&lt;/a&gt; of Nearly 4 Million Documents Associated with North Carolina &lt;a href="https://newsie.social/tags/Vaping" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Vaping&lt;/span&gt;&lt;/a&gt; Settlement, First 280K Docs Now Online &lt;a href="https://www.infodocket.com/2024/01/31/research-tools-unc-collaboration-to-create-public-depository-of-nearly-4-million-documents-associated-with-north-carolina-vaping-settlement-first-280k-now-online/" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;infodocket.com/2024/01/31/rese&lt;/span&gt;&lt;span class="invisible"&gt;arch-tools-unc-collaboration-to-create-public-depository-of-nearly-4-million-documents-associated-with-north-carolina-vaping-settlement-first-280k-now-online/&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>1.118528711378141e+17</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>SoLSec</t>
+        </is>
+      </c>
+      <c r="D388" s="2" t="n">
+        <v>45322.92785564815</v>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;What Apple&amp;#39;s Promise to Support RCS Means for Text Messaging &lt;a href="https://www.eff.org/deeplinks/2024/01/what-apples-promise-support-rcs-means-text-messaging" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;eff.org/deeplinks/2024/01/what&lt;/span&gt;&lt;span class="invisible"&gt;-apples-promise-support-rcs-means-text-messaging&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>1.118528711170357e+17</v>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D389" s="2" t="n">
+        <v>45322.92785197917</v>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Donations pour in to replace destroyed Jackie Robinson statue on his 105th birthday &lt;a href="https://my24group.com/donations-pour-in-to-replace-destroyed-jackie-robinson-statue-on-his-105th-birthday/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/donations-pour-i&lt;/span&gt;&lt;span class="invisible"&gt;n-to-replace-destroyed-jackie-robinson-statue-on-his-105th-birthday/&lt;/span&gt;&lt;/a&gt; Donations poured in Wednesday to replace a decimated statue of Jackie Robinson on what would have been the 105th birthday …&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>1.118528710745587e+17</v>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>austin_traffic_bot</t>
+        </is>
+      </c>
+      <c r="D390" s="2" t="n">
+        <v>45322.92784451389</v>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Crash Urgent at 1617 S Ih 35 Svrd Nb --- &lt;a href="https://www.google.com/maps/search/?api=1&amp;amp;query=30.24104%2C-97.736259" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;google.com/maps/search/?api=1&amp;amp;&lt;/span&gt;&lt;span class="invisible"&gt;query=30.24104%2C-97.736259&lt;/span&gt;&lt;/a&gt; --- &lt;a href="https://mastodon.social/tags/austin" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;austin&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/austintx" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;austintx&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/traffic" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;traffic&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="n">
+        <v>1.118528710657866e+17</v>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>aris</t>
+        </is>
+      </c>
+      <c r="D391" s="2" t="n">
+        <v>45322.92783564814</v>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;I reached the dangerous threshold in 99% of the projects I initiate where I got my dopamine high from getting a POC working and risk giving up the long term benefits of continuing the project to completion.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
+        <v>1.118528710503627e+17</v>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>ScienceScholar</t>
+        </is>
+      </c>
+      <c r="D392" s="2" t="n">
+        <v>45322.92784021991</v>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Narcissistic CEOs are bad for share value but good for company inertia, says study &lt;a href="https://phys.org/news/2024-01-narcissistic-ceos-bad-good-company.html" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;phys.org/news/2024-01-narcissi&lt;/span&gt;&lt;span class="invisible"&gt;stic-ceos-bad-good-company.html&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/science" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;science&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>1.118528710346902e+17</v>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D393" s="2" t="n">
+        <v>45322.92783743056</v>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Εκατοντάδες τρακτέρ θα κατακλύσουν τις Βρυξέλλες την ημέρα της Συνόδου Κορυφής | Η ΚΑΘΗΜΕΡΙΝΗ &lt;a href="https://my24group.com/ekatontades-trakter-tha-kataklysoyn-tis-vryxelles-tin-imera-tis-synodoy-koryfis-i-kathimerini/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/ekatontades-trak&lt;/span&gt;&lt;span class="invisible"&gt;ter-tha-kataklysoyn-tis-vryxelles-tin-imera-tis-synodoy-koryfis-i-kathimerini/&lt;/span&gt;&lt;/a&gt; Αρκετές εκατοντάδε&amp;amp;sigma…&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="n">
+        <v>1.118528710326103e+17</v>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>photocyte</t>
+        </is>
+      </c>
+      <c r="D394" s="2" t="n">
+        <v>45322.92782407408</v>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Huge thank you to the whole team: Vik Shende, Igor Wierzbicki (UCSD), Bob Auber (Purdue &amp;amp; beyond!), David Gonzalez (UCSD), Jen Wisecaver (@Purdue), and Brad Moore(@Scripps_Ocean). I’m so grateful we united combining mecha style to tackle this truly monster challenge. Maybe a candidate for &lt;a href="https://genomic.social/tags/monsterdon" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;monsterdon&lt;/span&gt;&lt;/a&gt; ?? 🧵7/n&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n">
+        <v>1.118528710302021e+17</v>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>modernghana</t>
+        </is>
+      </c>
+      <c r="D395" s="2" t="n">
+        <v>45322.92782407408</v>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;“Let no one feel discouraged to use the law — CJ to Judges&amp;nbsp; &lt;a href="https://www.modernghana.com/news/1289439/let-no-one-feel-discouraged-to-use-the-law-cj.html" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;modernghana.com/news/1289439/l&lt;/span&gt;&lt;span class="invisible"&gt;et-no-one-feel-discouraged-to-use-the-law-cj.html&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n">
+        <v>1.118528710160529e+17</v>
+      </c>
+      <c r="B396" t="inlineStr"/>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>ProdigalFrog</t>
+        </is>
+      </c>
+      <c r="D396" s="2" t="n">
+        <v>45322.927695</v>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The New Ryzen APUs so bad they make the 6500 XT look good | 3kliksphillip&lt;/p&gt;&lt;p&gt;&lt;a href="https://slrpnk.net/post/6301138" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;slrpnk.net/post/6301138&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="n">
+        <v>1.118528710126812e+17</v>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>AlexPed</t>
+        </is>
+      </c>
+      <c r="D397" s="2" t="n">
+        <v>45322.92778935185</v>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://mastodon.uno/tags/GoodNight" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;GoodNight&lt;/span&gt;&lt;/a&gt; 🌙✨&lt;/p&gt;&lt;p&gt;&lt;a href="https://mastodon.uno/tags/FediRadio" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;FediRadio&lt;/span&gt;&lt;/a&gt; 📻   &lt;/p&gt;&lt;p&gt;Malinconia d'ottobre - Lucio Dalla &lt;br&gt;&lt;a href="https://inv.nadeko.net/watch?v=a3_XlVhIqSI" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;inv.nadeko.net/watch?v=a3_XlVh&lt;/span&gt;&lt;span class="invisible"&gt;IqSI&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="n">
+        <v>1.118528709858372e+17</v>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>Apatapa</t>
+        </is>
+      </c>
+      <c r="D398" s="2" t="n">
+        <v>45322.92782407408</v>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;In a world of hyperconnectivity where our online motions are tracked and profited off of by corporate entities which gather more and more political and economic power over time I would like to highlight that logging off and reading a book is becoming increasingly punk&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="n">
+        <v>1.118528709656418e+17</v>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>mbompard</t>
+        </is>
+      </c>
+      <c r="D399" s="2" t="n">
+        <v>45322.9278125</v>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Une contribution utile à la réflexion.&lt;br&gt;&amp;lt;p&amp;gt;&lt;br&gt; &lt;a href="https://nitter.cz/AntoineSallesP/status/1752787555542561108#m" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;nitter.cz/AntoineSallesP/statu&lt;/span&gt;&lt;span class="invisible"&gt;s/1752787555542561108#m&lt;/span&gt;&lt;/a&gt;&lt;br&gt;&amp;lt;/p&amp;gt;&lt;/p&gt;&lt;p&gt; 🐦🔗: &lt;a href="https://nitter.cz/mbompard/status/1752796113357205641#m" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;nitter.cz/mbompard/status/1752&lt;/span&gt;&lt;span class="invisible"&gt;796113357205641#m&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;[2024-01-31 20:48 UTC]&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="n">
+        <v>1.118528709620958e+17</v>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D400" s="2" t="n">
+        <v>45322.92782473379</v>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Αγρότες «περικύκλωσαν» τις Βρυξέλλες με τρακτέρ – «Δεν θα φύγουμε αν δεν πάρουμε όσα ζητάμε» (βίντεο) &lt;a href="https://my24group.com/agrotes-perikyklosan-tis-vryxelles-me-trakter-den-tha-fygoyme-an-den-paroyme-osa-zitame-vinteo/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/agrotes-perikykl&lt;/span&gt;&lt;span class="invisible"&gt;osan-tis-vryxelles-me-trakter-den-tha-fygoyme-an-den-paroyme-osa-zitame-vinteo/&lt;/span&gt;&lt;/a&gt; Αρκετές εκατοντάδε&amp;amp;sigma…&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="n">
+        <v>1.118528709370833e+17</v>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>Sharr0w</t>
+        </is>
+      </c>
+      <c r="D401" s="2" t="n">
+        <v>45322.92780092593</v>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;like VAT avoidance isn't illegal, and all emailed from the company email, which is also their company domain and registered trade name.&lt;/p&gt;&lt;p&gt;So they are not VAT compliant, are avoiding taxes, which annoys me, esp when they try to make me complicit.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="n">
+        <v>1.118528727661583e+17</v>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>maxxaine</t>
+        </is>
+      </c>
+      <c r="D402" s="2" t="n">
+        <v>45322.92814324074</v>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://mastodon.social/tags/WeimArisierung" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;WeimArisierung&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="n">
+        <v>1.118528727263672e+17</v>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>photocyte</t>
+        </is>
+      </c>
+      <c r="D403" s="2" t="n">
+        <v>45322.92811342593</v>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Lastly, we’d love to hear your feedback and Qs. I'll read it all and aim to answer all that I can. Hope you enjoyed being amongst the first to hear about the PKZILLAs! Careful, giants can sneak up on ya, even if they're inside a tiny &lt;a href="https://genomic.social/tags/algal" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;algal&lt;/span&gt;&lt;/a&gt; / &lt;a href="https://genomic.social/tags/algae" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;algae&lt;/span&gt;&lt;/a&gt; cell… 🧵8/8 &lt;a href="https://genomic.social/tags/biochemistry" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;biochemistry&lt;/span&gt;&lt;/a&gt; &lt;a href="https://genomic.social/tags/genomics" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;genomics&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="n">
+        <v>1.118528726985531e+17</v>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>my24group</t>
+        </is>
+      </c>
+      <c r="D404" s="2" t="n">
+        <v>45322.92813127315</v>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Startup news site The Messenger shutters less than a year after its launch &lt;a href="https://my24group.com/startup-news-site-the-messenger-shutters-less-than-a-year-after-its-launch/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;my24group.com/startup-news-sit&lt;/span&gt;&lt;span class="invisible"&gt;e-the-messenger-shutters-less-than-a-year-after-its-launch/&lt;/span&gt;&lt;/a&gt; The news outlet promised to provide “thorough, objective, non-partisan, and timely news coverage” in a time of…&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="n">
+        <v>1.11852872695413e+17</v>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>su</t>
+        </is>
+      </c>
+      <c r="D405" s="2" t="n">
+        <v>45322.92811342593</v>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Nigger 2&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="n">
+        <v>1.118528726889907e+17</v>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>wsj</t>
+        </is>
+      </c>
+      <c r="D406" s="2" t="n">
+        <v>45322.92803240741</v>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Energy &amp;amp; Utilities Roundup: Market Talk:&lt;br&gt;Gain insight on Saudi Arabia’s oil capacity, GDP data for Canada, Transnet, and more in the latest Market Talks covering Energy and Utilities.&lt;br&gt;&lt;a href="https://www.wsj.com/articles/energy-utilities-roundup-market-talk-74ffe250" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;wsj.com/articles/energy-utilit&lt;/span&gt;&lt;span class="invisible"&gt;ies-roundup-market-talk-74ffe250&lt;/span&gt;&lt;/a&gt;&lt;br&gt;(Wed, 31 Jan 2024 17:09:00 -0500)&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="n">
+        <v>1.118528726726192e+17</v>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>dgar</t>
+        </is>
+      </c>
+      <c r="D407" s="2" t="n">
+        <v>45322.92805555555</v>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;So far, I've had some repairs done to the Strat, and it's working fine.&lt;/p&gt;&lt;p&gt;I have a new DI - a Focusrite Scarlett 2i2 Generation 4.  It's good.  Better than anything I've used before.&lt;/p&gt;&lt;p&gt;I have a new microphone.  Focusrite has a Studio package that includes a ribbon mic.  It seems so be fine.&lt;/p&gt;&lt;p&gt;I don't have a new computer yet.  I'm working on an external drive attached to my slowly dying iMac.  It's intolerably slow for Blender and absolutely unusable for Unreal Engine.  I'm trying to end my relationship with Adobe, so Blender will probably pick up the slack from leaving Illustrator.  My recent song Airlock has album art created in Blender.&lt;/p&gt;&lt;p&gt;Apple came out with their M3 series chips that have ray tracing.  Maybe they''ll release a decent desktop machine soon.&lt;/p&gt;&lt;p&gt;So the studio is up and running now, we're making progress and getting some work done.&lt;/p&gt;&lt;p&gt;Huzzah!&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="n">
+        <v>1.118528726414503e+17</v>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>RadarMechelen</t>
+        </is>
+      </c>
+      <c r="D408" s="2" t="n">
+        <v>45322.92812122685</v>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Flight: &lt;a href="https://mastodon.social/tags/WUK8622" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;WUK8622&lt;/span&gt;&lt;/a&gt;&lt;br /&gt;Registration: G-WUKG&lt;br /&gt;ICAO code: #407510&lt;br /&gt;Callsign: &lt;a href="https://mastodon.social/tags/WIZZ" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;WIZZ&lt;/span&gt;&lt;/a&gt; GO&lt;br /&gt;Operator: Wizz Air Uk&lt;br /&gt;Type: AIRBUS A321-231&lt;br /&gt;Country: 🇬🇧&lt;br /&gt;Speed: 697 kmh&lt;br /&gt;Altitude: 10988 m&lt;br /&gt;Distance: 7.2 km&lt;br /&gt;Angle ∆: 56.6°&lt;br /&gt;Direction -&amp;gt;: WNW&lt;br /&gt;Track:&lt;br /&gt;&lt;a href="http://globe.adsbexchange.com/?icao=407510&amp;amp;lat=50.983&amp;amp;lon=4.447&amp;amp;zoom=10.5&amp;amp;showTrace=2024-01-31" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;http://&lt;/span&gt;&lt;span class="ellipsis"&gt;globe.adsbexchange.com/?icao=4&lt;/span&gt;&lt;span class="invisible"&gt;07510&amp;amp;lat=50.983&amp;amp;lon=4.447&amp;amp;zoom=10.5&amp;amp;showTrace=2024-01-31&lt;/span&gt;&lt;/a&gt;&lt;br /&gt;&lt;a href="http://globe.adsb.fi/?icao=407510&amp;amp;lat=50.983&amp;amp;lon=4.447&amp;amp;zoom=10.5&amp;amp;showTrace=2024-01-31" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;http://&lt;/span&gt;&lt;span class="ellipsis"&gt;globe.adsb.fi/?icao=407510&amp;amp;lat&lt;/span&gt;&lt;span class="invisible"&gt;=50.983&amp;amp;lon=4.447&amp;amp;zoom=10.5&amp;amp;showTrace=2024-01-31&lt;/span&gt;&lt;/a&gt;&lt;br /&gt;History:&lt;br /&gt;&lt;a href="https://www.radarbox.com/data/mode-s/407510" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;radarbox.com/data/mode-s/40751&lt;/span&gt;&lt;span class="invisible"&gt;0&lt;/span&gt;&lt;/a&gt;&lt;br /&gt;&lt;a href="https://www.flightradar24.com/data/aircraft/G-WUKG" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;flightradar24.com/data/aircraf&lt;/span&gt;&lt;span class="invisible"&gt;t/G-WUKG&lt;/span&gt;&lt;/a&gt;&lt;br /&gt;Photos:&lt;br /&gt;&lt;a href="https://jetphotos.com/photo/keyword/G-WUKG" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;jetphotos.com/photo/keyword/G-&lt;/span&gt;&lt;span class="invisible"&gt;WUKG&lt;/span&gt;&lt;/a&gt;&lt;br /&gt;Seen: 40x&lt;br /&gt;&lt;a href="http://bit.ly/gift-for-radar-mechelen" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;http://&lt;/span&gt;&lt;span class=""&gt;bit.ly/gift-for-radar-mechelen&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="n">
+        <v>1.118528726396451e+17</v>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>ChicagoNewsBot</t>
+        </is>
+      </c>
+      <c r="D409" s="2" t="n">
+        <v>45322.92739583334</v>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Chicago shooting: 3 teens shot, seriously injured in Edgewater, fire officials say&lt;br&gt;       &lt;a href="https://abc7chicago.com/chicago-shooting-edgewater-three-teens-shot-crime/14375887/" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;abc7chicago.com/chicago-shooti&lt;/span&gt;&lt;span class="invisible"&gt;ng-edgewater-three-teens-shot-crime/14375887/&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="n">
+        <v>1.118528726342277e+17</v>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>Lazarou</t>
+        </is>
+      </c>
+      <c r="D410" s="2" t="n">
+        <v>45322.92811993056</v>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Elmo&amp;#39;s are emotional vampires who feed off human misery. Do not fall for their tricks&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="n">
+        <v>1.118528726180499e+17</v>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>Underdog__NBA</t>
+        </is>
+      </c>
+      <c r="D411" s="2" t="n">
+        <v>45322.92685185185</v>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Miles Bridges (elbow) available to play Wednesday.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="n">
+        <v>1.118528726139034e+17</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>bartolopietro1</t>
+        </is>
+      </c>
+      <c r="D412" s="2" t="n">
+        <v>45322.92810185185</v>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Se questa è Europa.&lt;br&gt;Ungheria 2024&lt;br&gt;&lt;a href="https://nitter.cz/search?q=%23IlariaSalis" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;nitter.cz/search?q=%23IlariaSa&lt;/span&gt;&lt;span class="invisible"&gt;lis&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt; 🐦🔗: &lt;a href="https://nitter.cz/bartolopietro1/status/1752756991842242742#m" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;nitter.cz/bartolopietro1/statu&lt;/span&gt;&lt;span class="invisible"&gt;s/1752756991842242742#m&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;[2024-01-31 18:13 UTC]&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="n">
+        <v>1.118528726041647e+17</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>qme</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>FCBfemeni</t>
+        </is>
+      </c>
+      <c r="D413" s="2" t="n">
+        <v>45322.92777777778</v>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;🔴⚪️⚔️🔵🔴&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="n">
+        <v>1.118528725781947e+17</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>madbarrister</t>
+        </is>
+      </c>
+      <c r="D414" s="2" t="n">
+        <v>45322.92811010416</v>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;We would stop doing vote counts like horseraces. Nobody is &amp;quot;pulling ahead&amp;quot; or &amp;quot;falling behind&amp;quot;.  You can wait a few more hours (or even a day) until all the votes are counted and then one winner announced.&lt;/p&gt;&lt;p&gt;&lt;a href="https://mastodon.social/tags/IfIRanTheWorld" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;IfIRanTheWorld&lt;/span&gt;&lt;/a&gt;&lt;br /&gt;&lt;a href="https://mastodon.social/tags/HashItOut" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;HashItOut&lt;/span&gt;&lt;/a&gt;&lt;br /&gt;&lt;a href="https://mastodon.social/tags/HashtagGames" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;HashtagGames&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="n">
+        <v>1.118528725642189e+17</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>quotejung</t>
+        </is>
+      </c>
+      <c r="D415" s="2" t="n">
+        <v>45322.9271875</v>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;You have 3 options:&lt;/p&gt;&lt;p&gt;- Do nothing and continue as before&lt;br&gt;- Read hundreds of books and get the most important ideas from them&lt;br&gt;- Get your copy of 100 Mental Models&lt;/p&gt;&lt;p&gt;TAP HERE and get your copy RIGHT NOW!&lt;/p&gt;&lt;p&gt;👇👇&lt;/p&gt;&lt;p&gt;&lt;a href="https://gumroad.com/a/288617587/AxfYH" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;gumroad.com/a/288617587/AxfYH&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="n">
+        <v>1.118528725625e+17</v>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>Underdog__NBA</t>
+        </is>
+      </c>
+      <c r="D416" s="2" t="n">
+        <v>45322.92679398148</v>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;LaMelo Ball (ankle) ruled out Wednesday.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="n">
+        <v>1.118528725455522e+17</v>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>wsj</t>
+        </is>
+      </c>
+      <c r="D417" s="2" t="n">
+        <v>45322.92802083334</v>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;New York Community Bancorp Stock Plunges 38%, Reigniting Fears for Regional Banks:&lt;br&gt;NYCB built up capital after acquiring most of the failed Signature Bank in last year’s crisis.&lt;br&gt;&lt;a href="https://www.wsj.com/articles/new-york-community-bancorp-stock-plunges-35-reigniting-fears-for-regional-banks-7bf74972" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;wsj.com/articles/new-york-comm&lt;/span&gt;&lt;span class="invisible"&gt;unity-bancorp-stock-plunges-35-reigniting-fears-for-regional-banks-7bf74972&lt;/span&gt;&lt;/a&gt;&lt;br&gt;(Wed, 31 Jan 2024 17:11:00 -0500)&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="n">
+        <v>1.118528725416254e+17</v>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>espn</t>
+        </is>
+      </c>
+      <c r="D418" s="2" t="n">
+        <v>45322.9016550926</v>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Álvarez brace leads Man City win over Burnley as Haaland returns&lt;br&gt;&lt;a href="https://www.espn.com/soccer/report/_/gameId/671250?utm_source=flipboard&amp;amp;utm_medium=activitypub" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;espn.com/soccer/report/_/gameI&lt;/span&gt;&lt;span class="invisible"&gt;d/671250?utm_source=flipboard&amp;amp;utm_medium=activitypub &lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Posted into Soccer&lt;br&gt;&lt;a href="https://flipboard.com/@espn/soccer-l6qk3v8fz?utm_source=flipboard&amp;amp;utm_medium=activitypub" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;flipboard.com/@espn/soccer-l6q&lt;/span&gt;&lt;span class="invisible"&gt;k3v8fz?utm_source=flipboard&amp;amp;utm_medium=activitypub &lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="n">
+        <v>1.118528725249504e+17</v>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>TheAthleticFC</t>
+        </is>
+      </c>
+      <c r="D419" s="2" t="n">
+        <v>45322.92659722222</v>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Jurgen Klopp wins his 200th Premier League game.&lt;/p&gt;&lt;p&gt;Liverpool beat Chelsea 4-1 at Anfield to move five points clear at the top of the Premier League table.&lt;/p&gt;&lt;p&gt;&lt;a href="https://twitter.com/hashtag/LFC" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;LFC&lt;/span&gt;&lt;/a&gt; | &lt;a href="https://twitter.com/hashtag/CFC" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;CFC&lt;/span&gt;&lt;/a&gt; | &lt;a href="https://twitter.com/hashtag/LIVCHE" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;LIVCHE&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="n">
+        <v>1.118528725246576e+17</v>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>NickVanExit</t>
+        </is>
+      </c>
+      <c r="D420" s="2" t="n">
+        <v>45322.92664351852</v>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Luka &amp;amp; Christian Wood played in 55 games together last year.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="n">
+        <v>1.118528725246105e+17</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>ko</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>silverkey</t>
+        </is>
+      </c>
+      <c r="D421" s="2" t="n">
+        <v>45322.92806712963</v>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Zenless Zone Zero - State of Play Announcement Video | PS5 Games &lt;a href="https://www.youtube.com/watch?v=If7LQKe3C2w" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;youtube.com/watch?v=If7LQKe3C2&lt;/span&gt;&lt;span class="invisible"&gt;w&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="n">
+        <v>1.118528725210973e+17</v>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>indie1023_playlist</t>
+        </is>
+      </c>
+      <c r="D422" s="2" t="n">
+        <v>45322.9280999537</v>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;3:15pm The Wire by Haim from Days Are Gone&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="n">
+        <v>1.118528724916149e+17</v>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>EBL2017</t>
+        </is>
+      </c>
+      <c r="D423" s="2" t="n">
+        <v>45322.92708333334</v>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;It feels like something special is brewing at Liverpool once again 🏆🏆🏆🏆&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="n">
+        <v>1.118528724752392e+17</v>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>ntsk</t>
+        </is>
+      </c>
+      <c r="D424" s="2" t="n">
+        <v>45322.92807870371</v>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;眠すぎるなあ&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="n">
+        <v>1.118528724737459e+17</v>
+      </c>
+      <c r="B425" t="inlineStr"/>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>z428</t>
+        </is>
+      </c>
+      <c r="D425" s="2" t="n">
+        <v>45322.92053240741</v>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>Nah an Mitternacht. Leere Straßen, leere Bahnen. Ein müder Radkurier fährt noch einmal Gerichte in einer orangefarbenen Kiste nach auswärts. In den hohen Luxuswohnungen wabert künstliches Licht, neben der Haltestelle sammeln sich die ersten Bewohner der Dunkelheit und irgendwie lebt das Viertel immer unent... &lt;a href="https://z428.micro.blog/2024/01/31/nah-an-mitternacht.html" rel="nofollow noopener noreferrer" target="_blank"&gt;z428.micro.blog&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="n">
+        <v>1.118528724631848e+17</v>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>dfwticket</t>
+        </is>
+      </c>
+      <c r="D426" s="2" t="n">
+        <v>45322.92715277777</v>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The Invasion visits with former NFL WR Steve Smith Sr at the East-West Shrine Bowl Hall of Fame induction  &lt;a href="https://post.futurimedia.com/ktck/playlist/38/listen-6967.html?cb=1706731458.076953" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;post.futurimedia.com/ktck/playlist/…&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="n">
+        <v>1.118528724330589e+17</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>Renatomancer</t>
+        </is>
+      </c>
+      <c r="D427" s="2" t="n">
+        <v>45322.92807870371</v>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://www.sportskeeda.com/pop-culture/why-protect-taylor-swift-trending-twitter-viral-ai-outrage-explored" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;sportskeeda.com/pop-culture/wh&lt;/span&gt;&lt;span class="invisible"&gt;y-protect-taylor-swift-trending-twitter-viral-ai-outrage-explored&lt;/span&gt;&lt;/a&gt; &lt;a href="https://vmst.io/tags/deepfakes" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;deepfakes&lt;/span&gt;&lt;/a&gt; &lt;a href="https://vmst.io/tags/ProtectTaylorSwift" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;ProtectTaylorSwift&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n">
+        <v>1.118528724251667e+17</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>jcmccaffrey</t>
+        </is>
+      </c>
+      <c r="D428" s="2" t="n">
+        <v>45322.92694444444</v>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Reminder: This ends in a few hours ⤵️&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n">
+        <v>1.118528724053545e+17</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>Volquest_On3</t>
+        </is>
+      </c>
+      <c r="D429" s="2" t="n">
+        <v>45322.92703703704</v>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The NCAA responds following attorney generals from Tennessee and Virginia filing federal lawsuit on Wednesday.&lt;/p&gt;&lt;p&gt;🔗&lt;a href="https://www.on3.com/teams/tennessee-volunteers/news/ncaa-investigation-tennessee-football-attourney-general-statement/" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;on3.com/teams/tennesse…&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n">
+        <v>1.118528724046092e+17</v>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>_Cainer</t>
+        </is>
+      </c>
+      <c r="D430" s="2" t="n">
+        <v>45322.92690972222</v>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The NCAA responds following attorney generals from Tennessee and Virginia filing federal lawsuit on Wednesday. &lt;/p&gt;&lt;p&gt;🔗&lt;a href="https://www.on3.com/teams/tennessee-volunteers/news/ncaa-investigation-tennessee-football-attourney-general-statement/" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;on3.com/teams/tennesse…&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="n">
+        <v>1.118528723960599e+17</v>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>wsj</t>
+        </is>
+      </c>
+      <c r="D431" s="2" t="n">
+        <v>45322.92800925926</v>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Judge Dismisses Disney's Suit Against Ron DeSantis:&lt;br&gt;The entertainment company had sued the Florida governor, accusing him of a “targeted campaign of government retaliation.”&lt;br&gt;&lt;a href="https://www.wsj.com/articles/judge-dismisses-disneys-suit-against-ron-desantis-6b7c044b" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;wsj.com/articles/judge-dismiss&lt;/span&gt;&lt;span class="invisible"&gt;es-disneys-suit-against-ron-desantis-6b7c044b&lt;/span&gt;&lt;/a&gt;&lt;br&gt;(Wed, 31 Jan 2024 17:11:00 -0500)&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="n">
+        <v>1.118528723705439e+17</v>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>jonoabroad</t>
+        </is>
+      </c>
+      <c r="D432" s="2" t="n">
+        <v>45322.92803240741</v>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;FUCK YEAH ME&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="n">
+        <v>1.118528723389985e+17</v>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>tjuanmarti</t>
+        </is>
+      </c>
+      <c r="D433" s="2" t="n">
+        <v>45322.92747685185</v>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;F5 Caso Bergvall al límite.&lt;/p&gt;&lt;p&gt;Tottenham aprieta…. pero el Barça tiene un gran aliado por solo UN DÍA. Y creo es lo que puede acabar vistiendo a Lucas de azulgrana! El culebrón se acaba en 24 horas.&lt;/p&gt;&lt;p&gt;Lo intento explicar aquí 👇&lt;/p&gt;&lt;p&gt;&lt;a href="https://www.sport.es/es/noticias/barca/caso-bergvall-incertidumbre-barca-24-horas-limite-97594869" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;sport.es/es/noticias/ba…&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="n">
+        <v>1.118528723159862e+17</v>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>barstoolsports</t>
+        </is>
+      </c>
+      <c r="D434" s="2" t="n">
+        <v>45322.92710648148</v>
+      </c>
+      <c r="E434" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The Swifties Are Hailing Colin Cowherd as Their King After He Defended Taylor's Airtime During Chiefs Games &lt;a href="https://www.barstoolsports.com/blog/3502077/the-swifties-are-hailing-colin-cowherd-as-their-king-after-he-defended-taylors-airtime-during-chiefs-games" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;barstoolsports.com/blog/3502077/t…&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="n">
+        <v>1.118528723065594e+17</v>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>Grafa</t>
+        </is>
+      </c>
+      <c r="D435" s="2" t="n">
+        <v>45322.92806207176</v>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Vinyl (ASX:VNL) closes acquisition of The Brag Media - published 31 Jan 2024 &lt;a href="https://mastodon.social/tags/Australia" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;Australia&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/News" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;News&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/ASX" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;ASX&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/Tech" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;Tech&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/Capital" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;Capital&lt;/span&gt;&lt;/a&gt; &lt;br /&gt;&lt;a href="https://grafa.com/news/vinyl--asx-vnl--closes-acquisition-of-the-brag-media-177198" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;grafa.com/news/vinyl--asx-vnl-&lt;/span&gt;&lt;span class="invisible"&gt;-closes-acquisition-of-the-brag-media-177198&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="n">
+        <v>1.118528723064921e+17</v>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>Eagles</t>
+        </is>
+      </c>
+      <c r="D436" s="2" t="n">
+        <v>45322.92708333334</v>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://twitter.com/hashtag/ProBowlGames" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;ProBowlGames&lt;/span&gt;&lt;/a&gt; had &lt;span class="h-card"&gt;&lt;a href="https://twitter.com/fcoxx_91" class="u-url mention" rel="nofollow noopener noreferrer" target="_blank"&gt;@&lt;span&gt;fcoxx_91@twitter.com&lt;/span&gt;&lt;/a&gt;&lt;/span&gt; acting DIFFERENT&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="n">
+        <v>1.118528723038044e+17</v>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>celtics</t>
+        </is>
+      </c>
+      <c r="D437" s="2" t="n">
+        <v>45322.92733796296</v>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://twitter.com/hashtag/NEBHInjuryReport" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NEBHInjuryReport&lt;/span&gt;&lt;/a&gt; for tomorrow vs. Los Angeles:&lt;/p&gt;&lt;p&gt;Luke Kornet (left hamstring strain) - QUESTIONABLE&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="n">
+        <v>1.118528722954757e+17</v>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>iembot_mtr</t>
+        </is>
+      </c>
+      <c r="D438" s="2" t="n">
+        <v>45322.92803240741</v>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://bots.krohsnest.com/tags/CAweather" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;CAweather&lt;/span&gt;&lt;/a&gt; &lt;a href="https://bots.krohsnest.com/tags/CAwx" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;CAwx&lt;/span&gt;&lt;/a&gt;&lt;br&gt;119 &lt;br&gt;NWUS56 KMTR 312211&lt;br&gt;LSRMTR&lt;/p&gt;&lt;p&gt;Preliminary Local Storm Report&lt;br&gt;National Weather Service San Francisco CA&lt;br&gt;211 PM PST Wed Jan 31 2024&lt;/p&gt;&lt;p&gt;..TIME...   ...EVENT...      ...CITY LOCATION...     ...LAT.LON...&lt;br&gt;..DATE...   ....MAG....      ..COUNTY LOCATION..ST.. ...SOURCE....&lt;br&gt;            ..REMARKS..&lt;/p&gt;&lt;p&gt;0154 PM     Non-Tstm Wnd Dmg 2 WSW Discovery Bay     37.90N 121.62W&lt;br&gt;01/31/2024                   Contra Cost &lt;a href="https://mesonet.agron.iastate.edu/lsr/#MTR/202401312154/202401312154" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;mesonet.agron.iastate.edu/lsr/&lt;/span&gt;&lt;span class="invisible"&gt;#MTR/202401312154/202401312154&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="n">
+        <v>1.118528722900806e+17</v>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>JacobsBen</t>
+        </is>
+      </c>
+      <c r="D439" s="2" t="n">
+        <v>45322.92674768518</v>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;FT: Liverpool 4 Chelsea 1. &lt;a href="https://twitter.com/hashtag/LFC" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;LFC&lt;/span&gt;&lt;/a&gt; exceptional, especially Bradley with a goal and two assists. They move five clear at the top of the Premier League. No doubt they deserved victory, even though &lt;a href="https://twitter.com/hashtag/CFC" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;CFC&lt;/span&gt;&lt;/a&gt; robbed of two clear penalties. Some very poor performances by the visitors.🔴🔵&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="n">
+        <v>1.118528722755217e+17</v>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>wsj</t>
+        </is>
+      </c>
+      <c r="D440" s="2" t="n">
+        <v>45322.92799768518</v>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Basic Materials Roundup: Market Talk:&lt;br&gt;Find insights on Ashland, Antofagasta, Transnet, and more in the latest latest Market Talks covering Basic Materials.&lt;br&gt;&lt;a href="https://www.wsj.com/articles/basic-materials-roundup-market-talk-6a891708" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;wsj.com/articles/basic-materia&lt;/span&gt;&lt;span class="invisible"&gt;ls-roundup-market-talk-6a891708&lt;/span&gt;&lt;/a&gt;&lt;br&gt;(Wed, 31 Jan 2024 17:12:00 -0500)&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="n">
+        <v>1.11852872268883e+17</v>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>quotejung</t>
+        </is>
+      </c>
+      <c r="D441" s="2" t="n">
+        <v>45322.9271875</v>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Control your MIND.&lt;/p&gt;&lt;p&gt;Work on Mental Models:&lt;br&gt;- Learn big ideas&lt;br&gt;- Study bug disciplines&lt;br&gt;- Strengthen your vision and leverage&lt;/p&gt;&lt;p&gt;Think in a multidisciplinary way.&lt;/p&gt;&lt;p&gt;(It has a money-back guarantee and is completely risk-free.)&lt;/p&gt;&lt;p&gt;Grab your copy here:&lt;/p&gt;&lt;p&gt;&lt;a href="https://gumroad.com/a/288617587/AxfYH" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;gumroad.com/a/288617587/AxfYH&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="n">
+        <v>1.118528751302362e+17</v>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>europesays</t>
+        </is>
+      </c>
+      <c r="D442" s="2" t="n">
+        <v>45322.92851851852</v>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://www.europesays.com/1031610/" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class=""&gt;europesays.com/1031610/&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt; Putin says earns $175K, owns couple of apartments and a parking spot &lt;a href="https://pubeurope.com/tags/europe" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;europe&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="n">
+        <v>1.118528750963491e+17</v>
+      </c>
+      <c r="B443" t="inlineStr"/>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>eff</t>
+        </is>
+      </c>
+      <c r="D443" s="2" t="n">
+        <v>45322.92786449074</v>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The good news: Apple’s Messages will soon support a number of basic features, like emoji reactions, with your green bubble friends. The bad news: those conversations could remain less secure until there is a standard for end-to-end encryption. &lt;a href="https://www.eff.org/deeplinks/2024/01/what-apples-promise-support-rcs-means-text-messaging" rel="nofollow noopener noreferrer" target="_blank"&gt;https://www.eff.org/deeplinks/2024/01/what-apples-promise-support-rcs-means-text-messaging&lt;/a&gt;&lt;/p&gt;&lt;p&gt; 🐦🔗: &lt;a href="https://nitter.oksocial.net/EFF/status/1752815777613565955#m" rel="nofollow noopener noreferrer" target="_blank"&gt;https://nitter.oksocial.net/EFF/status/1752815777613565955#m&lt;/a&gt;&lt;/p&gt;&lt;p&gt;[2024/01/31 22:07]&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="n">
+        <v>1.118528750954975e+17</v>
+      </c>
+      <c r="B444" t="inlineStr"/>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>kbin</t>
+        </is>
+      </c>
+      <c r="D444" s="2" t="n">
+        <v>45322.9284837963</v>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>#&lt;a class="" href="https://libera.site/search?tag=Kbin" rel="nofollow noopener noreferrer" target="_blank"&gt;Kbin&lt;/a&gt; #&lt;a class="" href="https://libera.site/search?tag=Statistics" rel="nofollow noopener noreferrer" target="_blank"&gt;Statistics&lt;/a&gt; 2024-01-31 23:00 CET&lt;br&gt;Number of active instances: 61&lt;br&gt;Number of users: 127 452&lt;br&gt;Number of posts: 256 925&lt;br&gt;Number of comments: 1 040 866&lt;br&gt;Number of new users last 2h: 4&lt;br&gt;Number of new posts last 2h: 27&lt;br&gt;Number of new comments last 2h: 243&lt;br&gt;      &lt;br&gt;#&lt;a class="" href="https://libera.site/search?tag=Fediverse" rel="nofollow noopener noreferrer" target="_blank"&gt;Fediverse&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="n">
+        <v>1.118528750782808e+17</v>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>livetapes</t>
+        </is>
+      </c>
+      <c r="D445" s="2" t="n">
+        <v>45322.92851851852</v>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The Cambodian Space Project @ Freiburg, Germany 2014-01-31 &lt;a href="https://ijwthstd.blogspot.com/2024/01/the-cambodian-space-project-freiburg.html" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;ijwthstd.blogspot.com/2024/01/&lt;/span&gt;&lt;span class="invisible"&gt;the-cambodian-space-project-freiburg.html&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="n">
+        <v>1.118528750662514e+17</v>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>LeoBurr</t>
+        </is>
+      </c>
+      <c r="D446" s="2" t="n">
+        <v>45322.9284837963</v>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;When the recipe calls for a clove of garlic.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="n">
+        <v>1.118528750003607e+17</v>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>rff</t>
+        </is>
+      </c>
+      <c r="D447" s="2" t="n">
+        <v>45322.9284837963</v>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Now playing on the radiofreefedi.net specialty channel:&lt;br&gt;&lt;br&gt;Cyberpsychosis by Revengeday &lt;a href="https://corteximplant.com/@revengeday" rel="nofollow noopener noreferrer" target="_blank"&gt;https://corteximplant.com/@revengeday&lt;/a&gt;&lt;br&gt;© used with permission&lt;br&gt;&lt;a href="https://revenge.day/" rel="nofollow noopener noreferrer" target="_blank"&gt;https://revenge.day/&lt;/a&gt;&lt;br&gt;&lt;br&gt;Tune in now: &lt;a href="https://radiofreefedi.net" rel="nofollow noopener noreferrer" target="_blank"&gt;https://radiofreefedi.net&lt;/a&gt;&lt;br&gt;interact with &lt;span class="h-card"&gt;&lt;a href="https://musician.social/@radiofreefedi" class="u-url mention" rel="nofollow noopener noreferrer" target="_blank"&gt;@&lt;span&gt;radiofreefedi&lt;/span&gt;&lt;/a&gt;&lt;/span&gt;&lt;br&gt;&lt;br&gt;your 24/7 community radio from the fediverse to the universe&lt;br&gt;&lt;a href="https://nowplaying.radiofreefedi.net/tags/rffplays" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;rffPlays&lt;/span&gt;&lt;/a&gt; &lt;a href="https://nowplaying.radiofreefedi.net/tags/rffspecialty" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;rffSpecialty&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="n">
+        <v>1.1185287488999e+17</v>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>nl</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>Portal4Cars</t>
+        </is>
+      </c>
+      <c r="D448" s="2" t="n">
+        <v>45322.92851831018</v>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Polestar 4 goes on sale in Europe and Australia with up to 379 miles WLTP range: The Polestar 4 officially hit two key markets Wednesday. Polestar launched its new SUV Coupe in Europe and Australia with up to 379 miles (610 km) WLTP range.   &lt;br /&gt;  &lt;br /&gt;  &lt;br /&gt;  &lt;br /&gt; more…&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="n">
+        <v>1.118528748759313e+17</v>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>KyleGCrider</t>
+        </is>
+      </c>
+      <c r="D449" s="2" t="n">
+        <v>45322.92850694444</v>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Professor recalls growing up in Birmingham public housing called ‘poorest ZIP code in America’ - al.com &lt;a href="https://www.al.com/news/2024/01/professor-recalls-growing-up-in-birmingham-public-housing-called-poorest-zip-code-in-america.html" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;al.com/news/2024/01/professor-&lt;/span&gt;&lt;span class="invisible"&gt;recalls-growing-up-in-birmingham-public-housing-called-poorest-zip-code-in-america.html&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="n">
+        <v>1.11852874813555e+17</v>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>riyapattnaik</t>
+        </is>
+      </c>
+      <c r="D450" s="2" t="n">
+        <v>45322.92850491898</v>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Hina Khan stresses on deep breaths while exercising: ‘Keeps you calm’&lt;/p&gt;&lt;p&gt;Hina Khan stresses on deep breaths while exercising: ‘Keeps you calm’. Image Source: IANS News Mumbai, Jan 31 : A fervent fitness enthusiast, actress Hina Khan&amp;#39;s holistic approach to exercise includes a focus on deep breaths, believing it not only enhances calmness but also boosts the ability to lift more. The &amp;#39;Yeh Rishta Kya Kehlata Hai&amp;#39; fame actress Hina, who enjoys 19 million followers on…&lt;/p&gt;&lt;p&gt;&lt;a href="https://www.ollywoodmovie.com/news/entertainment/9028/hina-khan-stresses-on-deep-breaths-while-exercising-keeps-you-calm/" target="_blank" rel="nofollow noopener noreferrer" translate="no"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;ollywoodmovie.com/news/enterta&lt;/span&gt;&lt;span class="invisible"&gt;inment/9028/hina-khan-stresses-on-deep-breaths-while-exercising-keeps-you-calm/&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="n">
+        <v>1.118528748095961e+17</v>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>ChrisShort</t>
+        </is>
+      </c>
+      <c r="D451" s="2" t="n">
+        <v>45322.9284837963</v>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Suggested Read: Heynote - &lt;a href="https://heynote.com/" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;heynote.com/&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt; &lt;a href="https://hachyderm.io/tags/devopsish" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;devopsish&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="n">
+        <v>1.118528747594625e+17</v>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>bullriders1</t>
+        </is>
+      </c>
+      <c r="D452" s="2" t="n">
+        <v>45322.9284837963</v>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;George Lynch 1987 🎸 &lt;a href="https://x.com/bullriders1/status/1752818105544577416?s=20" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;x.com/bullriders1/status/17528&lt;/span&gt;&lt;span class="invisible"&gt;18105544577416?s=20&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="n">
+        <v>1.118528746926419e+17</v>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>chamatou</t>
+        </is>
+      </c>
+      <c r="D453" s="2" t="n">
+        <v>45322.92847222222</v>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Pfou, cette chanson me faisait déjà de l'effet, mais je viens de lire les paroles et de voir le clip 🥲 Dire qu'elle n'a pas gagné l'Eurovision (mais elle remporté Sanremo) : &lt;a href="https://www.youtube.com/watch?v=22lISUXgSUw" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;youtube.com/watch?v=22lISUXgSU&lt;/span&gt;&lt;span class="invisible"&gt;w&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="n">
+        <v>1.118528746911858e+17</v>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>masainu</t>
+        </is>
+      </c>
+      <c r="D454" s="2" t="n">
+        <v>45322.9284375</v>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;F1がアンドレッティの2025年からの参戦を認めないと決定&lt;/p&gt;&lt;p&gt;F1、アンドレッティの2025年からの参戦を認めないと結論「この選手権に追加の価値をもたらさないと判断した」　しかし2028年参入の可能性は残す &lt;a href="https://jp.motorsport.com/f1/news/f1-rejects-andretti-entry-for-now-but-door-open-for-2028/10571091/" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;jp.motorsport.com/f1/news/f1-r&lt;/span&gt;&lt;span class="invisible"&gt;ejects-andretti-entry-for-now-but-door-open-for-2028/10571091/&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="n">
+        <v>1.118528746092423e+17</v>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>quotejung</t>
+        </is>
+      </c>
+      <c r="D455" s="2" t="n">
+        <v>45322.92721064815</v>
+      </c>
+      <c r="E455" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;100 Mental Models.&lt;/p&gt;&lt;p&gt;Different perspectives.&lt;/p&gt;&lt;p&gt;Different mindsets.&lt;/p&gt;&lt;p&gt;Different ways to achieve success.&lt;/p&gt;&lt;p&gt;Click here:&lt;/p&gt;&lt;p&gt;&lt;a href="https://gumroad.com/a/288617587/AxfYH" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;gumroad.com/a/288617587/AxfYH&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="n">
+        <v>1.118528745110141e+17</v>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>kuvo_playlist</t>
+        </is>
+      </c>
+      <c r="D456" s="2" t="n">
+        <v>45322.92845140046</v>
+      </c>
+      <c r="E456" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;3:16pm Yes I Can, No You Can&amp;#39;t by Lee Morgan from The Gigolo&lt;br /&gt;&lt;a href="https://mastodon.social/tags/LeeMorgan" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;LeeMorgan&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/YesICanNoYouCant" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;YesICanNoYouCant&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/MiddayJazz" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;MiddayJazz&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.social/tags/KUVO" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;KUVO&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="n">
+        <v>1.118528745017625e+17</v>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>craftykraken</t>
+        </is>
+      </c>
+      <c r="D457" s="2" t="n">
+        <v>45322.92841435185</v>
+      </c>
+      <c r="E457" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;yassss :hearthands: one of my favourite modern-day pianists, &lt;a href="https://mstdn.games/tags/HaniaRani" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;HaniaRani&lt;/span&gt;&lt;/a&gt; did a &lt;a href="https://mstdn.games/tags/tinydesk" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;tinydesk&lt;/span&gt;&lt;/a&gt; &lt;/p&gt;&lt;p&gt;&lt;a href="https://mstdn.games/tags/music" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;music&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mstdn.games/tags/piano" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;piano&lt;/span&gt;&lt;/a&gt; &lt;/p&gt;&lt;p&gt;&lt;a href="https://www.youtube.com/watch?v=4RcKtr5bGa4" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;youtube.com/watch?v=4RcKtr5bGa&lt;/span&gt;&lt;span class="invisible"&gt;4&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="n">
+        <v>1.118528744942382e+17</v>
+      </c>
+      <c r="B458" t="inlineStr"/>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>yolu</t>
+        </is>
+      </c>
+      <c r="D458" s="2" t="n">
+        <v>45322.92843677083</v>
+      </c>
+      <c r="E458" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;span&gt;よく寝た&lt;/span&gt;​:blob_yannya:​​:ohanyo:​&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="n">
+        <v>1.118528744626226e+17</v>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>GrantShowSwan</t>
+        </is>
+      </c>
+      <c r="D459" s="2" t="n">
+        <v>45322.92839120371</v>
+      </c>
+      <c r="E459" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Taylor Swift, Travis Kelce and a MAGA Meltdown &lt;a href="https://www.nytimes.com/2024/01/30/us/politics/taylor-swift-travis-kelce-trump.html?bgrp=c&amp;amp;smid=tw-share" rel="nofollow noopener noreferrer" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;nytimes.com/2024/01/30/us/poli&lt;/span&gt;&lt;span class="invisible"&gt;tics/taylor-swift-travis-kelce-trump.html?bgrp=c&amp;amp;smid=tw-share&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="n">
+        <v>1.118528744049081e+17</v>
+      </c>
+      <c r="B460" t="inlineStr"/>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="D460" s="2" t="n">
+        <v>45322.92837836806</v>
+      </c>
+      <c r="E460" t="inlineStr">
+        <is>
+          <t>四个译者没一个敢译哈姆雷特吃人，切，看我的&lt;br&gt;&lt;a href="https://vnil.de/media/8b57b1dd-98a0-4081-96a0-d0dcef4b88ff/image.png" class="" rel="nofollow noopener noreferrer" target="_blank"&gt; the funeral baked meats  Did c…&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="n">
+        <v>1.118528743825226e+17</v>
+      </c>
+      <c r="B461" t="inlineStr"/>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>takenoko</t>
+        </is>
+      </c>
+      <c r="D461" s="2" t="n">
+        <v>45322.92842265046</v>
+      </c>
+      <c r="E461" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;span&gt;朝飯食うかあ&lt;/span&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="n">
+        <v>1.11852874367407e+17</v>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>quotejung</t>
+        </is>
+      </c>
+      <c r="D462" s="2" t="n">
+        <v>45322.92719907407</v>
+      </c>
+      <c r="E462" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The most terrifying thing is to accept oneself completely.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="n">
+        <v>1.11852874316393e+17</v>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>NicolasMolli14</t>
+        </is>
+      </c>
+      <c r="D463" s="2" t="n">
+        <v>45322.92839120371</v>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://fr.motor1.com/news/706796/giottivictoria-nouvelle-marque-automobile-italie/" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;fr.motor1.com/news/706796/giot&lt;/span&gt;&lt;span class="invisible"&gt;tivictoria-nouvelle-marque-automobile-italie/&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;GiottiVictoria : la nouvelle marque automobile italienne présente 2 SUV d'origine chinoise.&lt;/p&gt;&lt;p&gt;&lt;a href="https://piaille.fr/tags/GiottiVictoria" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;GiottiVictoria&lt;/span&gt;&lt;/a&gt; &lt;br&gt;&lt;a href="https://piaille.fr/tags/Italie" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Italie&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n">
+        <v>1.118528742693792e+17</v>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>xl_ent</t>
+        </is>
+      </c>
+      <c r="D464" s="2" t="n">
+        <v>45322.92840872685</v>
+      </c>
+      <c r="E464" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://mastodon.social/tags/HalloliebeAutofahrer" class="mention hashtag" rel="tag"&gt;#&lt;span&gt;HalloliebeAutofahrer&lt;/span&gt;&lt;/a&gt;, die Post für Januar ist raus. Die guten Vorsätze waren eher so lalala von euch, oder?&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n">
+        <v>1.118528742649087e+17</v>
+      </c>
+      <c r="B465" t="inlineStr"/>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>fuyama</t>
+        </is>
+      </c>
+      <c r="D465" s="2" t="n">
+        <v>45322.92840465278</v>
+      </c>
+      <c r="E465" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;span&gt;興奮しすぎて細かい部分の記憶が曖昧になっている。今日は散らかった情緒をまとめる作業だな&lt;/span&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n">
+        <v>1.118528742544388e+17</v>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>aetherglow</t>
+        </is>
+      </c>
+      <c r="D466" s="2" t="n">
+        <v>45322.92838085648</v>
+      </c>
+      <c r="E466" t="inlineStr">
+        <is>
+          <t>&lt;span class="h-card"&gt;&lt;a class="u-url mention" href="https://social.translunar.academy/users/aetherglow" rel="nofollow noopener noreferrer" target="_blank"&gt;@&lt;span&gt;Aetherglow&lt;/span&gt;&lt;/a&gt;&lt;/span&gt;, an interactive story:&lt;br&gt;&lt;br&gt;&lt;a href="https://translunar.academy/fic/post/344" rel="nofollow noopener noreferrer" target="_blank"&gt;https://translunar.academy/fic/post/344&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n">
+        <v>1.118528741937368e+17</v>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>RaphMikey</t>
+        </is>
+      </c>
+      <c r="D467" s="2" t="n">
+        <v>45322.92839533565</v>
+      </c>
+      <c r="E467" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Thursday..  new orchid and new blooms...&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n">
+        <v>1.118528741862007e+17</v>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>scoub</t>
+        </is>
+      </c>
+      <c r="D468" s="2" t="n">
+        <v>45322.92837962963</v>
+      </c>
+      <c r="E468" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Gens de France ... à voir sur &lt;a href="https://mamot.fr/tags/Blast" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;Blast&lt;/span&gt;&lt;/a&gt; &lt;br&gt;40 ANS APRÈS LA MARCHE : MADANI, SES IMAGES ET LE MEPRIS&lt;br&gt;Madani Merzouk est un personnage important du quartier du Valdegour à Nîmes. À partir de l’année 1986, il filme tous les moments importants des actions culturelles et politiques de son quartier et en fait un documentaire : « S’hab la Zup. » À la fin des années 80, une poignée de leaders associatifs dynamisent la vie citoyenne des habitants de la cité nîmoise...&lt;br&gt;&lt;a href="https://www.blast-info.fr/emissions/2023/40-ans-apres-la-marche-madani-ses-images-et-le-mepris-asHcgOS9TS6jZTT3Mn_P-g" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;blast-info.fr/emissions/2023/4&lt;/span&gt;&lt;span class="invisible"&gt;0-ans-apres-la-marche-madani-ses-images-et-le-mepris-asHcgOS9TS6jZTT3Mn_P-g&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="n">
+        <v>1.118528741778125e+17</v>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>stopthatgirl7</t>
+        </is>
+      </c>
+      <c r="D469" s="2" t="n">
+        <v>45322.92837962963</v>
+      </c>
+      <c r="E469" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;A proposed Satanic school helped derail a vote to repeal Idaho's Blaine Amendment&lt;/p&gt;&lt;p&gt;If the bill succeeds, taxpayer dollars could be funneled to religious schools... including Satanic ones. &lt;/p&gt;&lt;p&gt;&lt;a href="https://www.friendlyatheist.com/p/a-proposed-satanic-school-helped" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;friendlyatheist.com/p/a-propos&lt;/span&gt;&lt;span class="invisible"&gt;ed-satanic-school-helped&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n">
+        <v>1.118528741303821e+17</v>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>irish_abroad</t>
+        </is>
+      </c>
+      <c r="D470" s="2" t="n">
+        <v>45322.92836805555</v>
+      </c>
+      <c r="E470" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;📋 &lt;span class="h-card" translate="no"&gt;&lt;a href="https://mastodon.ie/@irish_abroad" class="u-url mention" rel="nofollow noopener noreferrer" target="_blank"&gt;@&lt;span&gt;irish_abroad&lt;/span&gt;&lt;/a&gt;&lt;/span&gt; summary for Wednesday, 31 January 2024&lt;br&gt;🏃 10 starting players(4 substituted)&lt;br&gt;💺 5 substitutes(2 introduced)&lt;br&gt;🅰️ 1 assist&lt;br&gt;⚽ 3 goals&lt;br&gt;🟥 1 red card&lt;br&gt;⚽ 1 OG&lt;br&gt;All events and full lineups available on the live blog: &lt;a href="http://irish-abroad.appspot.com/Live" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;http://&lt;/span&gt;&lt;span class=""&gt;irish-abroad.appspot.com/Live&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;br&gt;&lt;a href="https://mastodon.ie/tags/COYGIG" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;COYGIG&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.ie/tags/COYBIG" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;COYBIG&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n">
+        <v>1.118528741228252e+17</v>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>soviet</t>
+        </is>
+      </c>
+      <c r="D471" s="2" t="n">
+        <v>45322.92835648148</v>
+      </c>
+      <c r="E471" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;The Charlatans - The Only One I Know&lt;br&gt;&lt;a href="https://youtu.be/0RJwW77Lsj8" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;youtu.be/0RJwW77Lsj8&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;br&gt;&lt;a href="https://lile.cl/tags/nowplaying" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;nowplaying&lt;/span&gt;&lt;/a&gt; &lt;a href="https://lile.cl/tags/music" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;music&lt;/span&gt;&lt;/a&gt; &lt;a href="https://lile.cl/tags/musica" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;musica&lt;/span&gt;&lt;/a&gt; &lt;a href="https://lile.cl/tags/musique" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;musique&lt;/span&gt;&lt;/a&gt; &lt;a href="https://lile.cl/tags/%D0%BC%D1%83%D0%B7%D1%8B%D0%BA%D0%B0" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;музыка&lt;/span&gt;&lt;/a&gt; &lt;a href="https://lile.cl/tags/musik" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;musik&lt;/span&gt;&lt;/a&gt; &lt;a href="https://lile.cl/tags/musikken" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;musikken&lt;/span&gt;&lt;/a&gt; &lt;a href="https://lile.cl/tags/thecharlatans" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;thecharlatans&lt;/span&gt;&lt;/a&gt; &lt;a href="https://lile.cl/tags/sovietmuzyka" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;sovietmuzyka&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n">
+        <v>1.118528741228252e+17</v>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>Sarb</t>
+        </is>
+      </c>
+      <c r="D472" s="2" t="n">
+        <v>45322.92834490741</v>
+      </c>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;In todays vlog, I’m in a hurry and I can't miss this ferry! Insta360 ace pro electric bike vlog&lt;br&gt;&lt;a href="https://youtu.be/GIE65vnCv5Y" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class=""&gt;youtu.be/GIE65vnCv5Y&lt;/span&gt;&lt;span class="invisible"&gt;&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n">
+        <v>1.118528741162568e+17</v>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>NATO_ACT</t>
+        </is>
+      </c>
+      <c r="D473" s="2" t="n">
+        <v>45322.92834490741</v>
+      </c>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://bots.defencegeeks.net/tags/NATO" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;NATO&lt;/span&gt;&lt;/a&gt;'s highly trained troops, ready to act against any potential threats in all domains with a wide range of capabilities &amp;amp; a steadfast commitment to defending its Allies!&lt;/p&gt;&lt;p&gt;📸@COM_SNMG2's team is sharpening their fast rope skills. &lt;/p&gt;&lt;p&gt;&lt;a href="https://bots.defencegeeks.net/tags/WeAreNATO" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;WeAreNATO&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Original tweet: &lt;a href="https://twitter.com/NATO_ACT/status/1752738794753708302" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;twitter.com/NATO_ACT/status/17&lt;/span&gt;&lt;span class="invisible"&gt;52738794753708302&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n">
+        <v>1.118528741131824e+17</v>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>kcqon</t>
+        </is>
+      </c>
+      <c r="D474" s="2" t="n">
+        <v>45322.92836805555</v>
+      </c>
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;It's going to be a busy KubeCon EU :-)&lt;/p&gt;&lt;p&gt;* eBPF Day: Falco, Tracee and Tetragon: eBPF Runtime Observability and Security Tools Differences&lt;/p&gt;&lt;p&gt;* KubeCon Day 2: Building a Tool to Debug Minimal Container Images in Kubernetes, Docker and ContainerD&lt;/p&gt;&lt;p&gt;* KubeCon Day 3: Contribfest: Making SlimToolkit Even Easier to Use: Building a Terminal UI&lt;/p&gt;&lt;p&gt; &lt;a href="https://infosec.exchange/tags/kubecon" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;kubecon&lt;/span&gt;&lt;/a&gt; &lt;a href="https://infosec.exchange/tags/cloudnativecon" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;cloudnativecon&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="n">
+        <v>1.118528741013337e+17</v>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>hachre</t>
+        </is>
+      </c>
+      <c r="D475" s="2" t="n">
+        <v>45322.9271875</v>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;&lt;a href="https://mastodon.hach.re/tags/twitter" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;twitter&lt;/span&gt;&lt;/a&gt; &lt;a href="https://mastodon.hach.re/tags/crosspost" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;crosspost&lt;/span&gt;&lt;/a&gt; by @1410_berlin@twitter.com:&lt;/p&gt;&lt;p&gt;Alleine, dass man "russisches Gas" als Alternative überhaupt erwähnt ist so dermaßen daneben.&lt;/p&gt;&lt;p&gt;Scheiß auf die Ukrainer:innen die gerade verrecken, hauptsache billiges Gas.&lt;/p&gt;&lt;p&gt;Überzeugt davon? Dann wählt Bewegung Wagenknecht-Putin.&lt;/p&gt;&lt;p&gt;&lt;a href="http://nitter.hach.re/1410_berlin/status/1751927131666313512#m" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;http://&lt;/span&gt;&lt;span class="ellipsis"&gt;nitter.hach.re/1410_berlin/sta&lt;/span&gt;&lt;span class="invisible"&gt;tus/1751927131666313512#m&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="n">
+        <v>1.118528740940998e+17</v>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>ichigaya2016</t>
+        </is>
+      </c>
+      <c r="D476" s="2" t="n">
+        <v>45322.92834490741</v>
+      </c>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;戦艦大和だったか武蔵も見つけるプロジェクトがあったような記憶&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="n">
+        <v>1.118528740892956e+17</v>
+      </c>
+      <c r="B477" t="inlineStr"/>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>lemmy</t>
+        </is>
+      </c>
+      <c r="D477" s="2" t="n">
+        <v>45322.92828703704</v>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>#&lt;a class="" href="https://libera.site/search?tag=Lemmy" rel="nofollow noopener noreferrer" target="_blank"&gt;Lemmy&lt;/a&gt; #&lt;a class="" href="https://libera.site/search?tag=Statistics" rel="nofollow noopener noreferrer" target="_blank"&gt;Statistics&lt;/a&gt; 2024-01-31 23:00 CET&lt;br&gt;Number of active instances: 1 126&lt;br&gt;Number of users: 2 396 312&lt;br&gt;Number of posts: 8 998 649&lt;br&gt;Number of comments: 18 179 066&lt;br&gt;Number of new users last 2h: 416&lt;br&gt;Number of new posts last 2h: 2768&lt;br&gt;Number of new comments last 2h: 2943&lt;br&gt;      &lt;br&gt;#&lt;a class="" href="https://libera.site/search?tag=Fediverse" rel="nofollow noopener noreferrer" target="_blank"&gt;Fediverse&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="n">
+        <v>1.118528739697988e+17</v>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>nl</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>NuOpRadio2</t>
+        </is>
+      </c>
+      <c r="D478" s="2" t="n">
+        <v>45322.92833333334</v>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Weather With You van Crowded House. Dit nummer draait tot 23:19:34.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="n">
+        <v>1.118528739477506e+17</v>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>gratefuldread</t>
+        </is>
+      </c>
+      <c r="D479" s="2" t="n">
+        <v>45322.92821759259</v>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Disabled People Are Not Fire Hazards &lt;a href="https://progressive.org/latest/disabled-people-are-not-fire-hazards-ervin-20240131/?utm_source=dlvr.it&amp;amp;utm_medium=mastodon" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://&lt;/span&gt;&lt;span class="ellipsis"&gt;progressive.org/latest/disable&lt;/span&gt;&lt;span class="invisible"&gt;d-people-are-not-fire-hazards-ervin-20240131/?utm_source=dlvr.it&amp;amp;utm_medium=mastodon&lt;/span&gt;&lt;/a&gt; - @TheProgressive &lt;a href="https://gratefuldread.masto.host/tags/progressive" class="mention hashtag" rel="nofollow noopener noreferrer" target="_blank"&gt;#&lt;span&gt;progressive&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n">
+        <v>1.118528739069842e+17</v>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>wsj</t>
+        </is>
+      </c>
+      <c r="D480" s="2" t="n">
+        <v>45322.928125</v>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Qualcomm Revenue Tops Estimates:&lt;br&gt;The company logged better-than-expected revenue in the latest quarter, led by growth in handsets and automotive.&lt;br&gt;&lt;a href="https://www.wsj.com/articles/qualcomm-1q-revenue-tops-estimates-on-growth-in-handsets-automotive-31f098c4" rel="nofollow noopener noreferrer" translate="no" target="_blank"&gt;&lt;span class="invisible"&gt;https://www.&lt;/span&gt;&lt;span class="ellipsis"&gt;wsj.com/articles/qualcomm-1q-r&lt;/span&gt;&lt;span class="invisible"&gt;evenue-tops-estimates-on-growth-in-handsets-automotive-31f098c4&lt;/span&gt;&lt;/a&gt;&lt;br&gt;(Wed, 31 Jan 2024 16:40:00 -0500)&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n">
+        <v>1.118528739037109e+17</v>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>abitofzen</t>
+        </is>
+      </c>
+      <c r="D481" s="2" t="n">
+        <v>45322.92833333334</v>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;"Learn to watch your drama unfold while at the same time knowing you are more than your drama" - Ram Dass&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>